<commit_message>
Add parameter for recording JONSWAP spectrum gamma value in extreme calculations
</commit_message>
<xml_diff>
--- a/dds/moorings.xlsx
+++ b/dds/moorings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="419" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="419"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Tables" sheetId="5" r:id="rId5"/>
     <sheet name="Valid Values" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1374" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1383" uniqueCount="489">
   <si>
     <t>Identifier</t>
   </si>
@@ -1484,19 +1484,38 @@
   </si>
   <si>
     <t>filter.lease_area</t>
+  </si>
+  <si>
+    <t>farm.max_gamma_100_year</t>
+  </si>
+  <si>
+    <t>Maximum JONSWAP gamma</t>
+  </si>
+  <si>
+    <t>JONSWAP gamma parameter at maximum wave conditions (100 year return period)</t>
+  </si>
+  <si>
+    <t>jonswap_gamma</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1589,28 +1608,28 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1623,8 +1642,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="40% - Accent3" xfId="2" builtinId="39"/>
@@ -1979,11 +1999,11 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:H65"/>
+  <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C31" sqref="C31"/>
+      <selection pane="topRight" activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2577,7 +2597,7 @@
       <c r="C36" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="D36" s="16" t="s">
+      <c r="D36" s="17" t="s">
         <v>115</v>
       </c>
       <c r="G36" s="16" t="s">
@@ -2585,34 +2605,31 @@
       </c>
     </row>
     <row r="37" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="16" t="s">
-        <v>116</v>
+      <c r="A37" s="17" t="s">
+        <v>485</v>
       </c>
       <c r="B37" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="D37" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="G37" s="16" t="s">
-        <v>98</v>
+      <c r="C37" s="17" t="s">
+        <v>486</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="38" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="16" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B38" s="16" t="s">
         <v>33</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G38" s="16" t="s">
         <v>98</v>
@@ -2620,16 +2637,16 @@
     </row>
     <row r="39" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="16" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B39" s="16" t="s">
         <v>33</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="G39" s="16" t="s">
         <v>98</v>
@@ -2637,277 +2654,277 @@
     </row>
     <row r="40" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="16" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B40" s="16" t="s">
         <v>33</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G40" s="16" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="41" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="B41" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C41" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="D41" s="15" t="s">
-        <v>130</v>
+    <row r="41" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="G41" s="16" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="42" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="15" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B42" s="15" t="s">
         <v>40</v>
       </c>
       <c r="C42" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C43" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="D42" s="15" t="s">
+      <c r="D43" s="15" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="B43" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C43" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="D43" s="16" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="44" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="16" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B44" s="16" t="s">
         <v>33</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="45" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="16" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B45" s="16" t="s">
         <v>33</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="46" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="16" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B46" s="16" t="s">
         <v>33</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>458</v>
-      </c>
-      <c r="G46" s="16" t="s">
-        <v>46</v>
+        <v>142</v>
       </c>
     </row>
     <row r="47" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="16" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>147</v>
+        <v>458</v>
+      </c>
+      <c r="G47" s="16" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="16" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B48" s="16" t="s">
         <v>37</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="49" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="16" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B49" s="16" t="s">
         <v>37</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="50" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="16" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B50" s="16" t="s">
         <v>37</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="51" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="16" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B51" s="16" t="s">
         <v>37</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="52" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="16" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B52" s="16" t="s">
         <v>37</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="53" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="16" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B53" s="16" t="s">
         <v>37</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D53" s="16" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="54" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="16" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>451</v>
+        <v>37</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D54" s="16" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="55" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="16" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>37</v>
+        <v>451</v>
       </c>
       <c r="C55" s="16" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D55" s="16" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="56" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A56" s="16" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B56" s="16" t="s">
         <v>37</v>
       </c>
       <c r="C56" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="D56" s="16" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="B57" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C57" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="D56" s="16" t="s">
+      <c r="D57" s="16" t="s">
         <v>174</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="H57" s="3" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="58" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="H58" s="3" t="s">
         <v>178</v>
@@ -2915,119 +2932,136 @@
     </row>
     <row r="59" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>180</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>183</v>
+        <v>455</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="H59" s="3" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>180</v>
       </c>
       <c r="C60" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="H60" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A61" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C61" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="D61" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3"/>
-      <c r="G60" s="3"/>
-    </row>
-    <row r="61" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="16" t="s">
-        <v>188</v>
-      </c>
-      <c r="B61" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C61" s="16" t="s">
-        <v>189</v>
-      </c>
-      <c r="D61" s="16" t="s">
-        <v>190</v>
-      </c>
-      <c r="G61" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="H61" s="16" t="s">
-        <v>178</v>
-      </c>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
     </row>
     <row r="62" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="B62" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C62" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="D62" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="G62" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="H62" s="16" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="B62" s="16" t="s">
+      <c r="B63" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C62" s="16" t="s">
+      <c r="C63" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="D62" s="16" t="s">
+      <c r="D63" s="16" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="63" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="3" t="s">
+    <row r="64" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="3" t="s">
         <v>194</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A64" s="3" t="s">
-        <v>197</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>180</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
-      <c r="G64" s="3"/>
+        <v>196</v>
+      </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>180</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>456</v>
+        <v>198</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
       <c r="G65" s="3"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A66" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -3817,10 +3851,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:Q62"/>
+  <dimension ref="A1:Q63"/>
   <sheetViews>
     <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4257,15 +4291,15 @@
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>119</v>
-      </c>
-      <c r="B38" t="s">
+        <v>485</v>
+      </c>
+      <c r="B38" s="11" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B39" t="s">
         <v>298</v>
@@ -4273,7 +4307,7 @@
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B40" t="s">
         <v>298</v>
@@ -4281,7 +4315,7 @@
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B41" t="s">
         <v>298</v>
@@ -4289,7 +4323,7 @@
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B42" t="s">
         <v>298</v>
@@ -4297,7 +4331,7 @@
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B43" t="s">
         <v>298</v>
@@ -4305,7 +4339,7 @@
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B44" t="s">
         <v>298</v>
@@ -4313,59 +4347,23 @@
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
+        <v>137</v>
+      </c>
+      <c r="B45" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>140</v>
       </c>
-      <c r="B45" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A46" s="8" t="s">
-        <v>145</v>
-      </c>
       <c r="B46" t="s">
-        <v>299</v>
-      </c>
-      <c r="C46" t="s">
-        <v>299</v>
-      </c>
-      <c r="D46" t="s">
-        <v>299</v>
-      </c>
-      <c r="E46" t="s">
-        <v>298</v>
-      </c>
-      <c r="F46" t="s">
-        <v>299</v>
-      </c>
-      <c r="G46" t="s">
-        <v>298</v>
-      </c>
-      <c r="H46" t="s">
-        <v>298</v>
-      </c>
-      <c r="I46" t="s">
-        <v>298</v>
-      </c>
-      <c r="J46" t="s">
-        <v>298</v>
-      </c>
-      <c r="K46" t="s">
-        <v>298</v>
-      </c>
-      <c r="L46" t="s">
-        <v>298</v>
-      </c>
-      <c r="M46" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="N46" s="8" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" s="8" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B47" t="s">
         <v>299</v>
@@ -4400,23 +4398,16 @@
       <c r="L47" t="s">
         <v>298</v>
       </c>
-      <c r="M47" t="s">
-        <v>298</v>
-      </c>
-      <c r="N47" t="s">
-        <v>298</v>
-      </c>
-      <c r="O47" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="P47" s="8" t="s">
-        <v>301</v>
-      </c>
-      <c r="Q47" s="8"/>
+      <c r="M47" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="N47" s="8" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B48" t="s">
         <v>299</v>
@@ -4451,16 +4442,23 @@
       <c r="L48" t="s">
         <v>298</v>
       </c>
-      <c r="M48" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="N48" s="8" t="s">
-        <v>301</v>
-      </c>
+      <c r="M48" t="s">
+        <v>298</v>
+      </c>
+      <c r="N48" t="s">
+        <v>298</v>
+      </c>
+      <c r="O48" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="P48" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="Q48" s="8"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A49" s="8" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B49" t="s">
         <v>299</v>
@@ -4504,7 +4502,7 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A50" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B50" t="s">
         <v>299</v>
@@ -4533,16 +4531,22 @@
       <c r="J50" t="s">
         <v>298</v>
       </c>
-      <c r="K50" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="L50" s="8" t="s">
+      <c r="K50" t="s">
+        <v>298</v>
+      </c>
+      <c r="L50" t="s">
+        <v>298</v>
+      </c>
+      <c r="M50" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="N50" s="8" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A51" s="8" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B51" t="s">
         <v>299</v>
@@ -4571,22 +4575,16 @@
       <c r="J51" t="s">
         <v>298</v>
       </c>
-      <c r="K51" t="s">
-        <v>302</v>
-      </c>
-      <c r="L51" t="s">
-        <v>302</v>
-      </c>
-      <c r="M51" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="N51" s="8" t="s">
+      <c r="K51" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="L51" s="8" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A52" s="8" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B52" t="s">
         <v>299</v>
@@ -4630,27 +4628,51 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A53" s="8" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B53" t="s">
         <v>299</v>
       </c>
-      <c r="C53" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>298</v>
+      <c r="C53" t="s">
+        <v>299</v>
+      </c>
+      <c r="D53" t="s">
+        <v>299</v>
       </c>
       <c r="E53" t="s">
         <v>298</v>
       </c>
       <c r="F53" t="s">
-        <v>298</v>
+        <v>299</v>
+      </c>
+      <c r="G53" t="s">
+        <v>298</v>
+      </c>
+      <c r="H53" t="s">
+        <v>298</v>
+      </c>
+      <c r="I53" t="s">
+        <v>298</v>
+      </c>
+      <c r="J53" t="s">
+        <v>298</v>
+      </c>
+      <c r="K53" t="s">
+        <v>302</v>
+      </c>
+      <c r="L53" t="s">
+        <v>302</v>
+      </c>
+      <c r="M53" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="N53" s="8" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>172</v>
+      <c r="A54" s="8" t="s">
+        <v>169</v>
       </c>
       <c r="B54" t="s">
         <v>299</v>
@@ -4670,71 +4692,47 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="B55" t="s">
         <v>299</v>
       </c>
-      <c r="C55" t="s">
-        <v>298</v>
-      </c>
-      <c r="D55" t="s">
+      <c r="C55" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="D55" s="8" t="s">
         <v>298</v>
       </c>
       <c r="E55" t="s">
-        <v>303</v>
+        <v>298</v>
+      </c>
+      <c r="F55" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B56" t="s">
         <v>299</v>
       </c>
       <c r="C56" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D56" t="s">
         <v>298</v>
       </c>
       <c r="E56" t="s">
-        <v>298</v>
-      </c>
-      <c r="F56" t="s">
-        <v>298</v>
-      </c>
-      <c r="G56" t="s">
-        <v>298</v>
-      </c>
-      <c r="H56" t="s">
-        <v>298</v>
-      </c>
-      <c r="I56" t="s">
-        <v>298</v>
-      </c>
-      <c r="J56" t="s">
-        <v>298</v>
-      </c>
-      <c r="K56" t="s">
-        <v>298</v>
-      </c>
-      <c r="L56" t="s">
-        <v>299</v>
-      </c>
-      <c r="M56" t="s">
-        <v>298</v>
-      </c>
-      <c r="N56" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B57" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C57" t="s">
         <v>299</v>
@@ -4743,97 +4741,141 @@
         <v>298</v>
       </c>
       <c r="E57" t="s">
+        <v>298</v>
+      </c>
+      <c r="F57" t="s">
+        <v>298</v>
+      </c>
+      <c r="G57" t="s">
+        <v>298</v>
+      </c>
+      <c r="H57" t="s">
+        <v>298</v>
+      </c>
+      <c r="I57" t="s">
+        <v>298</v>
+      </c>
+      <c r="J57" t="s">
+        <v>298</v>
+      </c>
+      <c r="K57" t="s">
+        <v>298</v>
+      </c>
+      <c r="L57" t="s">
         <v>299</v>
+      </c>
+      <c r="M57" t="s">
+        <v>298</v>
+      </c>
+      <c r="N57" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
+        <v>185</v>
+      </c>
+      <c r="B58" t="s">
+        <v>298</v>
+      </c>
+      <c r="C58" t="s">
+        <v>299</v>
+      </c>
+      <c r="D58" t="s">
+        <v>298</v>
+      </c>
+      <c r="E58" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
         <v>188</v>
-      </c>
-      <c r="B58" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A59" s="8" t="s">
-        <v>191</v>
       </c>
       <c r="B59" t="s">
         <v>299</v>
       </c>
-      <c r="C59" t="s">
-        <v>299</v>
-      </c>
-      <c r="D59" t="s">
-        <v>299</v>
-      </c>
-      <c r="E59" t="s">
-        <v>298</v>
-      </c>
-      <c r="F59" t="s">
-        <v>299</v>
-      </c>
-      <c r="G59" t="s">
-        <v>298</v>
-      </c>
-      <c r="H59" t="s">
-        <v>298</v>
-      </c>
-      <c r="I59" t="s">
-        <v>298</v>
-      </c>
-      <c r="J59" t="s">
-        <v>298</v>
-      </c>
-      <c r="K59" t="s">
-        <v>298</v>
-      </c>
-      <c r="L59" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="M59" s="8" t="s">
-        <v>301</v>
-      </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A60" s="8" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B60" t="s">
         <v>299</v>
       </c>
       <c r="C60" t="s">
-        <v>303</v>
+        <v>299</v>
+      </c>
+      <c r="D60" t="s">
+        <v>299</v>
+      </c>
+      <c r="E60" t="s">
+        <v>298</v>
+      </c>
+      <c r="F60" t="s">
+        <v>299</v>
+      </c>
+      <c r="G60" t="s">
+        <v>298</v>
+      </c>
+      <c r="H60" t="s">
+        <v>298</v>
+      </c>
+      <c r="I60" t="s">
+        <v>298</v>
+      </c>
+      <c r="J60" t="s">
+        <v>298</v>
+      </c>
+      <c r="K60" t="s">
+        <v>298</v>
+      </c>
+      <c r="L60" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="M60" s="8" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>197</v>
+      <c r="A61" s="8" t="s">
+        <v>194</v>
       </c>
       <c r="B61" t="s">
         <v>299</v>
       </c>
       <c r="C61" t="s">
-        <v>299</v>
-      </c>
-      <c r="D61" t="s">
-        <v>298</v>
-      </c>
-      <c r="E61" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B62" t="s">
         <v>299</v>
       </c>
       <c r="C62" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D62" t="s">
+        <v>298</v>
+      </c>
+      <c r="E62" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>200</v>
+      </c>
+      <c r="B63" t="s">
+        <v>299</v>
+      </c>
+      <c r="C63" t="s">
+        <v>298</v>
+      </c>
+      <c r="D63" t="s">
         <v>298</v>
       </c>
     </row>
@@ -4850,8 +4892,8 @@
   </sheetPr>
   <dimension ref="A1:Q44"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5641,10 +5683,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:Q53"/>
+  <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5941,105 +5983,90 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>116</v>
+        <v>485</v>
       </c>
       <c r="B24" t="s">
         <v>484</v>
       </c>
       <c r="C24" t="s">
-        <v>354</v>
+        <v>488</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B25" t="s">
         <v>484</v>
       </c>
       <c r="C25" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>125</v>
+      </c>
+      <c r="B26" t="s">
+        <v>484</v>
+      </c>
+      <c r="C26" t="s">
         <v>355</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>465</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="8" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B27" s="12" t="s">
         <v>465</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="8" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>465</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="12" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>465</v>
+      </c>
+      <c r="C29" t="s">
         <v>358</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>6</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>466</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>359</v>
-      </c>
-      <c r="D29" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>467</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>361</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>362</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>363</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>364</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>365</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>366</v>
+        <v>466</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>359</v>
+      </c>
+      <c r="D30" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>361</v>
@@ -6062,254 +6089,227 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>469</v>
-      </c>
-      <c r="C32" s="12" t="s">
+        <v>468</v>
+      </c>
+      <c r="C32" s="6" t="s">
         <v>361</v>
       </c>
-      <c r="D32" s="12" t="s">
-        <v>367</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>368</v>
+      <c r="D32" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>363</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>364</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>470</v>
-      </c>
-      <c r="C33" t="s">
-        <v>359</v>
+        <v>469</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>361</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>369</v>
-      </c>
-      <c r="E33" t="s">
-        <v>360</v>
-      </c>
-      <c r="F33" t="s">
-        <v>370</v>
-      </c>
-      <c r="G33" t="s">
-        <v>371</v>
+        <v>367</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C34" t="s">
-        <v>372</v>
+        <v>359</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E34" t="s">
-        <v>374</v>
+        <v>360</v>
       </c>
       <c r="F34" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="G34" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C35" t="s">
         <v>372</v>
       </c>
-      <c r="D35" t="s">
-        <v>377</v>
+      <c r="D35" s="12" t="s">
+        <v>373</v>
       </c>
       <c r="E35" t="s">
-        <v>378</v>
+        <v>374</v>
+      </c>
+      <c r="F35" t="s">
+        <v>375</v>
+      </c>
+      <c r="G35" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>472</v>
+      </c>
+      <c r="C36" t="s">
+        <v>372</v>
+      </c>
+      <c r="D36" t="s">
+        <v>377</v>
+      </c>
+      <c r="E36" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>29</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B37" s="12" t="s">
         <v>473</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>379</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>380</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E37" t="s">
         <v>381</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F37" t="s">
         <v>382</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G37" t="s">
         <v>383</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H37" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A37" s="7" t="s">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A38" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B37" s="12" t="s">
+      <c r="B38" s="12" t="s">
         <v>474</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C38" s="12" t="s">
         <v>385</v>
       </c>
-      <c r="D37" s="12" t="s">
+      <c r="D38" s="12" t="s">
         <v>386</v>
       </c>
-      <c r="E37" s="12" t="s">
+      <c r="E38" s="12" t="s">
         <v>387</v>
       </c>
-      <c r="F37" s="12" t="s">
+      <c r="F38" s="12" t="s">
         <v>388</v>
       </c>
-      <c r="G37" s="13" t="s">
+      <c r="G38" s="13" t="s">
         <v>389</v>
       </c>
-      <c r="H37" s="13" t="s">
+      <c r="H38" s="13" t="s">
         <v>390</v>
       </c>
-      <c r="I37" s="12" t="s">
+      <c r="I38" s="12" t="s">
         <v>391</v>
       </c>
-      <c r="J37" s="12" t="s">
+      <c r="J38" s="12" t="s">
         <v>392</v>
       </c>
-      <c r="K37" s="12" t="s">
+      <c r="K38" s="12" t="s">
         <v>340</v>
       </c>
-      <c r="L37" s="12" t="s">
+      <c r="L38" s="12" t="s">
         <v>393</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A38" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="B38" t="s">
-        <v>475</v>
-      </c>
-      <c r="C38" t="s">
-        <v>394</v>
-      </c>
-      <c r="D38" t="s">
-        <v>395</v>
-      </c>
-      <c r="E38" t="s">
-        <v>396</v>
-      </c>
-      <c r="F38" t="s">
-        <v>397</v>
-      </c>
-      <c r="G38" t="s">
-        <v>398</v>
-      </c>
-      <c r="H38" t="s">
-        <v>399</v>
-      </c>
-      <c r="I38" t="s">
-        <v>400</v>
-      </c>
-      <c r="J38" t="s">
-        <v>401</v>
-      </c>
-      <c r="K38" t="s">
-        <v>402</v>
-      </c>
-      <c r="L38" s="14" t="s">
-        <v>403</v>
-      </c>
-      <c r="M38" t="s">
-        <v>404</v>
-      </c>
-      <c r="N38" s="14" t="s">
-        <v>405</v>
-      </c>
-      <c r="O38" s="8" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="B39" s="12" t="s">
-        <v>476</v>
-      </c>
-      <c r="C39" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B39" t="s">
+        <v>475</v>
+      </c>
+      <c r="C39" t="s">
         <v>394</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D39" t="s">
         <v>395</v>
       </c>
-      <c r="E39" s="8" t="s">
+      <c r="E39" t="s">
         <v>396</v>
       </c>
-      <c r="F39" s="8" t="s">
+      <c r="F39" t="s">
         <v>397</v>
       </c>
-      <c r="G39" s="8" t="s">
+      <c r="G39" t="s">
         <v>398</v>
       </c>
-      <c r="H39" s="8" t="s">
+      <c r="H39" t="s">
         <v>399</v>
       </c>
-      <c r="I39" s="8" t="s">
+      <c r="I39" t="s">
         <v>400</v>
       </c>
       <c r="J39" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="K39" t="s">
-        <v>408</v>
-      </c>
-      <c r="L39" t="s">
-        <v>409</v>
-      </c>
-      <c r="M39" s="8" t="s">
-        <v>410</v>
+        <v>402</v>
+      </c>
+      <c r="L39" s="14" t="s">
+        <v>403</v>
+      </c>
+      <c r="M39" t="s">
+        <v>404</v>
       </c>
       <c r="N39" s="14" t="s">
-        <v>411</v>
-      </c>
-      <c r="O39" s="14" t="s">
-        <v>412</v>
-      </c>
-      <c r="P39" s="8" t="s">
-        <v>413</v>
-      </c>
-      <c r="Q39" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="O39" s="8" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>477</v>
+        <v>148</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>476</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>394</v>
@@ -6332,33 +6332,37 @@
       <c r="I40" s="8" t="s">
         <v>400</v>
       </c>
-      <c r="J40" s="8" t="s">
-        <v>401</v>
-      </c>
-      <c r="K40" s="8" t="s">
-        <v>402</v>
-      </c>
-      <c r="L40" s="14" t="s">
-        <v>403</v>
+      <c r="J40" t="s">
+        <v>407</v>
+      </c>
+      <c r="K40" t="s">
+        <v>408</v>
+      </c>
+      <c r="L40" t="s">
+        <v>409</v>
       </c>
       <c r="M40" s="8" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
       <c r="N40" s="14" t="s">
-        <v>405</v>
-      </c>
-      <c r="O40" s="8" t="s">
+        <v>411</v>
+      </c>
+      <c r="O40" s="14" t="s">
+        <v>412</v>
+      </c>
+      <c r="P40" s="8" t="s">
+        <v>413</v>
+      </c>
+      <c r="Q40" s="8" t="s">
         <v>406</v>
       </c>
-      <c r="P40" s="8"/>
-      <c r="Q40" s="8"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="B41" s="12" t="s">
-        <v>478</v>
+        <v>151</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>477</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>394</v>
@@ -6376,16 +6380,16 @@
         <v>398</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>414</v>
+        <v>399</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>415</v>
+        <v>400</v>
       </c>
       <c r="J41" s="8" t="s">
         <v>401</v>
       </c>
       <c r="K41" s="8" t="s">
-        <v>416</v>
+        <v>402</v>
       </c>
       <c r="L41" s="14" t="s">
         <v>403</v>
@@ -6399,13 +6403,15 @@
       <c r="O41" s="8" t="s">
         <v>406</v>
       </c>
+      <c r="P41" s="8"/>
+      <c r="Q41" s="8"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>157</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>479</v>
+      <c r="A42" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>478</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>394</v>
@@ -6423,30 +6429,36 @@
         <v>398</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>399</v>
+        <v>414</v>
       </c>
       <c r="I42" s="8" t="s">
+        <v>415</v>
+      </c>
+      <c r="J42" s="8" t="s">
         <v>401</v>
       </c>
-      <c r="J42" s="14" t="s">
+      <c r="K42" s="8" t="s">
+        <v>416</v>
+      </c>
+      <c r="L42" s="14" t="s">
         <v>403</v>
       </c>
-      <c r="K42" s="8" t="s">
+      <c r="M42" s="8" t="s">
         <v>404</v>
       </c>
-      <c r="L42" s="14" t="s">
+      <c r="N42" s="14" t="s">
         <v>405</v>
       </c>
-      <c r="M42" s="8" t="s">
+      <c r="O42" s="8" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A43" s="8" t="s">
-        <v>160</v>
+      <c r="A43" t="s">
+        <v>157</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>394</v>
@@ -6467,33 +6479,27 @@
         <v>399</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>400</v>
-      </c>
-      <c r="J43" s="8" t="s">
         <v>401</v>
       </c>
+      <c r="J43" s="14" t="s">
+        <v>403</v>
+      </c>
       <c r="K43" s="8" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="L43" s="14" t="s">
-        <v>411</v>
-      </c>
-      <c r="M43" s="14" t="s">
-        <v>412</v>
-      </c>
-      <c r="N43" s="8" t="s">
-        <v>413</v>
-      </c>
-      <c r="O43" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="M43" s="8" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" s="8" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>394</v>
@@ -6535,12 +6541,12 @@
         <v>406</v>
       </c>
     </row>
-    <row r="45" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" s="8" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>394</v>
@@ -6561,119 +6567,143 @@
         <v>399</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>417</v>
+        <v>400</v>
       </c>
       <c r="J45" s="8" t="s">
         <v>401</v>
       </c>
-      <c r="K45" s="14" t="s">
+      <c r="K45" s="8" t="s">
+        <v>402</v>
+      </c>
+      <c r="L45" s="14" t="s">
+        <v>411</v>
+      </c>
+      <c r="M45" s="14" t="s">
+        <v>412</v>
+      </c>
+      <c r="N45" s="8" t="s">
+        <v>413</v>
+      </c>
+      <c r="O45" s="8" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>482</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>397</v>
+      </c>
+      <c r="G46" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="H46" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="I46" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="J46" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="K46" s="14" t="s">
         <v>403</v>
       </c>
-      <c r="L45" s="8" t="s">
+      <c r="L46" s="8" t="s">
         <v>404</v>
       </c>
-      <c r="M45" s="14" t="s">
+      <c r="M46" s="14" t="s">
         <v>405</v>
       </c>
-      <c r="N45" s="8" t="s">
+      <c r="N46" s="8" t="s">
         <v>406</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>72</v>
-      </c>
-      <c r="B46" t="s">
-        <v>463</v>
-      </c>
-      <c r="C46" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>55</v>
-      </c>
-      <c r="B47" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47" t="s">
         <v>463</v>
       </c>
       <c r="C47" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>463</v>
       </c>
       <c r="C48" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>166</v>
+        <v>65</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>479</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>394</v>
-      </c>
-      <c r="D49" t="s">
-        <v>421</v>
+        <v>463</v>
+      </c>
+      <c r="C49" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>188</v>
+        <v>166</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>463</v>
-      </c>
-      <c r="C50" t="s">
-        <v>422</v>
+        <v>479</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="D50" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>97</v>
-      </c>
-      <c r="B51" t="s">
-        <v>484</v>
+        <v>188</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>463</v>
       </c>
       <c r="C51" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>169</v>
-      </c>
-      <c r="B52" s="12" t="s">
-        <v>483</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>424</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>425</v>
-      </c>
-      <c r="E52" s="8" t="s">
-        <v>426</v>
-      </c>
-      <c r="F52" s="8" t="s">
-        <v>427</v>
-      </c>
-      <c r="G52" s="8" t="s">
-        <v>428</v>
+        <v>97</v>
+      </c>
+      <c r="B52" t="s">
+        <v>484</v>
+      </c>
+      <c r="C52" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B53" s="12" t="s">
         <v>483</v>
@@ -6681,16 +6711,39 @@
       <c r="C53" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" s="8" t="s">
+        <v>425</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>426</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="G53" s="8" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>172</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>483</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>424</v>
+      </c>
+      <c r="D54" t="s">
         <v>429</v>
       </c>
-      <c r="E53" s="8" t="s">
+      <c r="E54" s="8" t="s">
         <v>430</v>
       </c>
-      <c r="F53" s="8" t="s">
+      <c r="F54" s="8" t="s">
         <v>431</v>
       </c>
-      <c r="G53" s="8" t="s">
+      <c r="G54" s="8" t="s">
         <v>432</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update device subsytems, components, equipment, ports and vessel dataspace.
</commit_message>
<xml_diff>
--- a/dds/moorings.xlsx
+++ b/dds/moorings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="419" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="419" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="472">
   <si>
     <t>Identifier</t>
   </si>
@@ -611,15 +611,6 @@
     <t>Friction Angle Sand-Pile</t>
   </si>
   <si>
-    <t>Maximum Bearing Capacity Factor</t>
-  </si>
-  <si>
-    <t>Maximum Unit Skin Friction</t>
-  </si>
-  <si>
-    <t>Maximum End Bearing Capacity</t>
-  </si>
-  <si>
     <t>Allowable Deflection / Diameter</t>
   </si>
   <si>
@@ -695,9 +686,6 @@
     <t>Material</t>
   </si>
   <si>
-    <t>Minimum Break Load</t>
-  </si>
-  <si>
     <t>Axial Stiffness</t>
   </si>
   <si>
@@ -749,9 +737,6 @@
     <t>Extension</t>
   </si>
   <si>
-    <t>% of Minimum Breaking Load</t>
-  </si>
-  <si>
     <t>Holding Capacity Coefficient 1</t>
   </si>
   <si>
@@ -1151,9 +1136,6 @@
     <t>moor_found_current_profile</t>
   </si>
   <si>
-    <t>fk_component_id</t>
-  </si>
-  <si>
     <t>sand_holding_cap_coef_1</t>
   </si>
   <si>
@@ -1316,9 +1298,6 @@
     <t>reference.view_component_moorings_swivel</t>
   </si>
   <si>
-    <t>reference.component_anchor</t>
-  </si>
-  <si>
     <t>filter.lease_area</t>
   </si>
   <si>
@@ -1455,6 +1434,24 @@
   </si>
   <si>
     <t>Euro/kg</t>
+  </si>
+  <si>
+    <t>reference.view_component_foundations_anchor_coefs</t>
+  </si>
+  <si>
+    <t>Max Bearing Capacity Factor</t>
+  </si>
+  <si>
+    <t>Max Unit Skin Friction</t>
+  </si>
+  <si>
+    <t>Max End Bearing Capacity</t>
+  </si>
+  <si>
+    <t>Min Break Load</t>
+  </si>
+  <si>
+    <t>% of Min Breaking Load</t>
   </si>
 </sst>
 </file>
@@ -2006,8 +2003,8 @@
   <dimension ref="A1:H65"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A2" sqref="A2:XFD2"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2037,10 +2034,10 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
@@ -2152,7 +2149,7 @@
         <v>147</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>148</v>
@@ -2195,7 +2192,7 @@
     </row>
     <row r="12" spans="1:8" s="15" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="15" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>6</v>
@@ -2209,7 +2206,7 @@
     </row>
     <row r="13" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>9</v>
@@ -2223,7 +2220,7 @@
     </row>
     <row r="14" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>9</v>
@@ -2237,7 +2234,7 @@
     </row>
     <row r="15" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>9</v>
@@ -2251,7 +2248,7 @@
     </row>
     <row r="16" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="15" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>9</v>
@@ -2269,7 +2266,7 @@
     </row>
     <row r="17" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="15" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>9</v>
@@ -2283,7 +2280,7 @@
     </row>
     <row r="18" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="15" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>9</v>
@@ -2297,7 +2294,7 @@
     </row>
     <row r="19" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="15" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>9</v>
@@ -2311,7 +2308,7 @@
     </row>
     <row r="20" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="15" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="B20" s="15" t="s">
         <v>26</v>
@@ -2487,7 +2484,7 @@
         <v>65</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
@@ -2507,7 +2504,7 @@
         <v>67</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="G31" s="15" t="s">
         <v>33</v>
@@ -2544,7 +2541,7 @@
         <v>73</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="G33" s="15" t="s">
         <v>33</v>
@@ -2558,10 +2555,10 @@
         <v>24</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="G34" s="15" t="s">
         <v>33</v>
@@ -2578,7 +2575,7 @@
         <v>125</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="G35" s="15" t="s">
         <v>33</v>
@@ -2657,16 +2654,16 @@
     </row>
     <row r="40" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="16" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="B40" s="15" t="s">
         <v>24</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="E40" s="15"/>
       <c r="F40" s="15"/>
@@ -2823,7 +2820,7 @@
     </row>
     <row r="49" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="17" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
       <c r="B49" s="15" t="s">
         <v>24</v>
@@ -2832,7 +2829,7 @@
         <v>25</v>
       </c>
       <c r="D49" s="18" t="s">
-        <v>442</v>
+        <v>435</v>
       </c>
     </row>
     <row r="50" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
@@ -2887,13 +2884,13 @@
     </row>
     <row r="53" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="20" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="B53" s="14" t="s">
         <v>24</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="D53" s="14" t="s">
         <v>29</v>
@@ -2905,7 +2902,7 @@
     </row>
     <row r="54" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="14" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="B54" s="14" t="s">
         <v>24</v>
@@ -2925,7 +2922,7 @@
     </row>
     <row r="55" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>159</v>
@@ -2945,7 +2942,7 @@
     </row>
     <row r="56" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>159</v>
@@ -2960,7 +2957,7 @@
     </row>
     <row r="57" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A57" s="19" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="B57" s="14" t="s">
         <v>28</v>
@@ -2978,7 +2975,7 @@
     </row>
     <row r="58" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="19" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="B58" s="14" t="s">
         <v>28</v>
@@ -2996,7 +2993,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" s="19" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="B59" s="14" t="s">
         <v>28</v>
@@ -3014,7 +3011,7 @@
     </row>
     <row r="60" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>159</v>
@@ -3032,13 +3029,13 @@
     </row>
     <row r="61" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>159</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>172</v>
@@ -3050,13 +3047,13 @@
     </row>
     <row r="62" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>159</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>160</v>
@@ -3067,13 +3064,13 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>156</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>157</v>
@@ -3087,7 +3084,7 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>159</v>
@@ -3104,13 +3101,13 @@
     </row>
     <row r="65" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A65" s="19" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="B65" s="14" t="s">
         <v>30</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="D65" s="14" t="s">
         <v>31</v>
@@ -3138,9 +3135,9 @@
   </sheetPr>
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="topRight" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3200,40 +3197,40 @@
         <v>129</v>
       </c>
       <c r="B2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E2" t="s">
+        <v>224</v>
+      </c>
+      <c r="F2" t="s">
+        <v>225</v>
+      </c>
+      <c r="G2" t="s">
+        <v>226</v>
+      </c>
+      <c r="H2" t="s">
+        <v>227</v>
+      </c>
+      <c r="I2" t="s">
+        <v>228</v>
+      </c>
+      <c r="J2" t="s">
+        <v>470</v>
+      </c>
+      <c r="K2" t="s">
         <v>216</v>
       </c>
-      <c r="C2" t="s">
-        <v>217</v>
-      </c>
-      <c r="D2" t="s">
-        <v>227</v>
-      </c>
-      <c r="E2" t="s">
-        <v>228</v>
-      </c>
-      <c r="F2" t="s">
-        <v>229</v>
-      </c>
-      <c r="G2" t="s">
-        <v>230</v>
-      </c>
-      <c r="H2" t="s">
-        <v>231</v>
-      </c>
-      <c r="I2" t="s">
-        <v>232</v>
-      </c>
-      <c r="J2" t="s">
-        <v>219</v>
-      </c>
-      <c r="K2" t="s">
-        <v>220</v>
-      </c>
       <c r="L2" s="13" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="Q2" s="6"/>
     </row>
@@ -3242,19 +3239,19 @@
         <v>150</v>
       </c>
       <c r="B3" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="E3" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="F3" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
@@ -3262,19 +3259,19 @@
         <v>153</v>
       </c>
       <c r="B4" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="E4" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="F4" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
@@ -3282,34 +3279,34 @@
         <v>135</v>
       </c>
       <c r="B5" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C5" t="s">
+        <v>214</v>
+      </c>
+      <c r="D5" t="s">
         <v>217</v>
       </c>
-      <c r="D5" t="s">
-        <v>221</v>
-      </c>
       <c r="E5" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F5" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="G5" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="H5" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="I5" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
@@ -3317,34 +3314,34 @@
         <v>126</v>
       </c>
       <c r="B6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D6" t="s">
+        <v>217</v>
+      </c>
+      <c r="E6" t="s">
+        <v>218</v>
+      </c>
+      <c r="F6" t="s">
+        <v>219</v>
+      </c>
+      <c r="G6" t="s">
+        <v>220</v>
+      </c>
+      <c r="H6" t="s">
+        <v>470</v>
+      </c>
+      <c r="I6" t="s">
         <v>216</v>
       </c>
-      <c r="C6" t="s">
-        <v>217</v>
-      </c>
-      <c r="D6" t="s">
-        <v>221</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="J6" s="13" t="s">
+        <v>461</v>
+      </c>
+      <c r="K6" s="13" t="s">
         <v>222</v>
-      </c>
-      <c r="F6" t="s">
-        <v>223</v>
-      </c>
-      <c r="G6" t="s">
-        <v>224</v>
-      </c>
-      <c r="H6" t="s">
-        <v>219</v>
-      </c>
-      <c r="I6" t="s">
-        <v>220</v>
-      </c>
-      <c r="J6" s="13" t="s">
-        <v>468</v>
-      </c>
-      <c r="K6" s="13" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
@@ -3352,34 +3349,34 @@
         <v>132</v>
       </c>
       <c r="B7" t="s">
+        <v>213</v>
+      </c>
+      <c r="C7" t="s">
+        <v>214</v>
+      </c>
+      <c r="D7" t="s">
+        <v>217</v>
+      </c>
+      <c r="E7" t="s">
+        <v>218</v>
+      </c>
+      <c r="F7" t="s">
+        <v>219</v>
+      </c>
+      <c r="G7" t="s">
+        <v>220</v>
+      </c>
+      <c r="H7" t="s">
+        <v>470</v>
+      </c>
+      <c r="I7" t="s">
         <v>216</v>
       </c>
-      <c r="C7" t="s">
-        <v>217</v>
-      </c>
-      <c r="D7" t="s">
-        <v>221</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="J7" s="13" t="s">
+        <v>461</v>
+      </c>
+      <c r="K7" s="13" t="s">
         <v>222</v>
-      </c>
-      <c r="F7" t="s">
-        <v>223</v>
-      </c>
-      <c r="G7" t="s">
-        <v>224</v>
-      </c>
-      <c r="H7" t="s">
-        <v>219</v>
-      </c>
-      <c r="I7" t="s">
-        <v>220</v>
-      </c>
-      <c r="J7" s="13" t="s">
-        <v>468</v>
-      </c>
-      <c r="K7" s="13" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
@@ -3387,31 +3384,31 @@
         <v>138</v>
       </c>
       <c r="B8" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D8" t="s">
         <v>217</v>
       </c>
-      <c r="D8" t="s">
-        <v>221</v>
-      </c>
       <c r="E8" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="F8" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G8" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="H8" t="s">
-        <v>219</v>
+        <v>470</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.35">
@@ -3419,13 +3416,13 @@
         <v>147</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>237</v>
+        <v>471</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.35">
@@ -3433,34 +3430,34 @@
         <v>141</v>
       </c>
       <c r="B10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C10" t="s">
+        <v>214</v>
+      </c>
+      <c r="D10" t="s">
+        <v>217</v>
+      </c>
+      <c r="E10" t="s">
+        <v>218</v>
+      </c>
+      <c r="F10" t="s">
+        <v>227</v>
+      </c>
+      <c r="G10" t="s">
+        <v>228</v>
+      </c>
+      <c r="H10" t="s">
+        <v>470</v>
+      </c>
+      <c r="I10" t="s">
         <v>216</v>
       </c>
-      <c r="C10" t="s">
-        <v>217</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="J10" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="E10" t="s">
+      <c r="K10" s="8" t="s">
         <v>222</v>
-      </c>
-      <c r="F10" t="s">
-        <v>231</v>
-      </c>
-      <c r="G10" t="s">
-        <v>232</v>
-      </c>
-      <c r="H10" t="s">
-        <v>219</v>
-      </c>
-      <c r="I10" t="s">
-        <v>220</v>
-      </c>
-      <c r="J10" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.35">
@@ -3468,39 +3465,39 @@
         <v>144</v>
       </c>
       <c r="B11" t="s">
+        <v>213</v>
+      </c>
+      <c r="C11" t="s">
+        <v>214</v>
+      </c>
+      <c r="D11" t="s">
+        <v>217</v>
+      </c>
+      <c r="E11" t="s">
+        <v>218</v>
+      </c>
+      <c r="F11" t="s">
+        <v>227</v>
+      </c>
+      <c r="G11" t="s">
+        <v>228</v>
+      </c>
+      <c r="H11" t="s">
+        <v>470</v>
+      </c>
+      <c r="I11" t="s">
         <v>216</v>
       </c>
-      <c r="C11" t="s">
-        <v>217</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="J11" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="E11" t="s">
+      <c r="K11" s="13" t="s">
         <v>222</v>
-      </c>
-      <c r="F11" t="s">
-        <v>231</v>
-      </c>
-      <c r="G11" t="s">
-        <v>232</v>
-      </c>
-      <c r="H11" t="s">
-        <v>219</v>
-      </c>
-      <c r="I11" t="s">
-        <v>220</v>
-      </c>
-      <c r="J11" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="K11" s="13" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="B12" t="s">
         <v>180</v>
@@ -3511,7 +3508,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>182</v>
@@ -3543,7 +3540,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="B14" t="s">
         <v>182</v>
@@ -3566,7 +3563,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="B15" t="s">
         <v>182</v>
@@ -3580,7 +3577,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="B16" t="s">
         <v>180</v>
@@ -3589,225 +3586,225 @@
         <v>190</v>
       </c>
       <c r="D16" t="s">
-        <v>191</v>
+        <v>467</v>
       </c>
       <c r="E16" t="s">
-        <v>192</v>
+        <v>468</v>
       </c>
       <c r="F16" t="s">
-        <v>193</v>
+        <v>469</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="B17" t="s">
+        <v>191</v>
+      </c>
+      <c r="C17" t="s">
+        <v>192</v>
+      </c>
+      <c r="D17" t="s">
+        <v>193</v>
+      </c>
+      <c r="E17" t="s">
         <v>194</v>
       </c>
-      <c r="C17" t="s">
+      <c r="F17" t="s">
         <v>195</v>
-      </c>
-      <c r="D17" t="s">
-        <v>196</v>
-      </c>
-      <c r="E17" t="s">
-        <v>197</v>
-      </c>
-      <c r="F17" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="B18" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C18" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D18" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="B19" t="s">
+        <v>198</v>
+      </c>
+      <c r="C19" t="s">
+        <v>199</v>
+      </c>
+      <c r="D19" t="s">
+        <v>200</v>
+      </c>
+      <c r="E19" t="s">
         <v>201</v>
       </c>
-      <c r="C19" t="s">
+      <c r="F19" t="s">
         <v>202</v>
       </c>
-      <c r="D19" t="s">
+      <c r="G19" t="s">
         <v>203</v>
-      </c>
-      <c r="E19" t="s">
-        <v>204</v>
-      </c>
-      <c r="F19" t="s">
-        <v>205</v>
-      </c>
-      <c r="G19" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="B20" t="s">
+        <v>204</v>
+      </c>
+      <c r="C20" t="s">
+        <v>205</v>
+      </c>
+      <c r="D20" t="s">
+        <v>206</v>
+      </c>
+      <c r="E20" t="s">
         <v>207</v>
       </c>
-      <c r="C20" t="s">
+      <c r="F20" t="s">
         <v>208</v>
       </c>
-      <c r="D20" t="s">
+      <c r="G20" t="s">
         <v>209</v>
       </c>
-      <c r="E20" t="s">
+      <c r="H20" t="s">
         <v>210</v>
       </c>
-      <c r="F20" t="s">
+      <c r="I20" t="s">
         <v>211</v>
-      </c>
-      <c r="G20" t="s">
-        <v>212</v>
-      </c>
-      <c r="H20" t="s">
-        <v>213</v>
-      </c>
-      <c r="I20" t="s">
-        <v>214</v>
       </c>
       <c r="J20" t="s">
         <v>25</v>
       </c>
       <c r="K20" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="B21" t="s">
+        <v>239</v>
+      </c>
+      <c r="C21" t="s">
+        <v>240</v>
+      </c>
+      <c r="D21" t="s">
+        <v>241</v>
+      </c>
+      <c r="E21" t="s">
+        <v>242</v>
+      </c>
+      <c r="F21" t="s">
+        <v>224</v>
+      </c>
+      <c r="G21" t="s">
+        <v>243</v>
+      </c>
+      <c r="H21" t="s">
+        <v>223</v>
+      </c>
+      <c r="I21" t="s">
+        <v>225</v>
+      </c>
+      <c r="J21" t="s">
         <v>244</v>
       </c>
-      <c r="C21" t="s">
+      <c r="K21" t="s">
         <v>245</v>
       </c>
-      <c r="D21" t="s">
+      <c r="L21" t="s">
         <v>246</v>
       </c>
-      <c r="E21" t="s">
+      <c r="M21" t="s">
         <v>247</v>
       </c>
-      <c r="F21" t="s">
-        <v>228</v>
-      </c>
-      <c r="G21" t="s">
+      <c r="N21" t="s">
         <v>248</v>
-      </c>
-      <c r="H21" t="s">
-        <v>227</v>
-      </c>
-      <c r="I21" t="s">
-        <v>229</v>
-      </c>
-      <c r="J21" t="s">
-        <v>249</v>
-      </c>
-      <c r="K21" t="s">
-        <v>250</v>
-      </c>
-      <c r="L21" t="s">
-        <v>251</v>
-      </c>
-      <c r="M21" t="s">
-        <v>252</v>
-      </c>
-      <c r="N21" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="B22" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="C22" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D22" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="E22" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="B23" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C23" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="B24" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C24" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="D24" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="B25" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C25" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D25" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="E25" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="B26" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C26" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="D26" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="E26" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -3843,22 +3840,22 @@
         <v>173</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>259</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>261</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>262</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>263</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.35">
@@ -3866,40 +3863,40 @@
         <v>129</v>
       </c>
       <c r="B2" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C2" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D2" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="E2" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="F2" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="G2" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="H2" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="I2" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="J2" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="K2" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="O2" s="13"/>
       <c r="P2" s="13"/>
@@ -3910,19 +3907,19 @@
         <v>150</v>
       </c>
       <c r="B3" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="E3" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="F3" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
@@ -3930,19 +3927,19 @@
         <v>153</v>
       </c>
       <c r="B4" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="E4" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="F4" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.35">
@@ -3950,34 +3947,34 @@
         <v>135</v>
       </c>
       <c r="B5" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C5" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D5" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="E5" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="F5" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="G5" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="H5" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="I5" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="M5" s="13"/>
       <c r="N5" s="13"/>
@@ -3987,34 +3984,34 @@
         <v>126</v>
       </c>
       <c r="B6" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C6" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D6" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="E6" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="F6" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="G6" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="H6" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="I6" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
@@ -4024,34 +4021,34 @@
         <v>132</v>
       </c>
       <c r="B7" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C7" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D7" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="E7" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="F7" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="G7" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="H7" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="I7" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="K7" s="13" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="M7" s="13"/>
       <c r="N7" s="13"/>
@@ -4061,31 +4058,31 @@
         <v>138</v>
       </c>
       <c r="B8" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C8" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D8" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="E8" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="F8" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="G8" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="H8" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
@@ -4095,34 +4092,34 @@
         <v>141</v>
       </c>
       <c r="B9" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C9" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D9" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="E9" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="F9" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="G9" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="H9" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="I9" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="K9" s="13" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="M9" s="13"/>
       <c r="N9" s="13"/>
@@ -4132,47 +4129,47 @@
         <v>144</v>
       </c>
       <c r="B10" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C10" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D10" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="E10" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="F10" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="G10" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="H10" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="I10" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="K10" s="13" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="M10" s="13"/>
       <c r="N10" s="13"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -4195,174 +4192,174 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="B12" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C12" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D12" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="E12" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="F12" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="G12" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="B13" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C13" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D13" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="E13" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="F13" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="G13" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="B14" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C14" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D14" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="B15" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C15" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D15" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="E15" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="F15" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="B16" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C16" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D16" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="E16" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="F16" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="B17" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C17" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D17" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="B18" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C18" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D18" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="E18" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="F18" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="G18" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="B19" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C19" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D19" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="E19" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="F19" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="G19" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="H19" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="I19" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="J19" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="K19" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
@@ -4370,7 +4367,7 @@
         <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
@@ -4378,7 +4375,7 @@
         <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
@@ -4386,7 +4383,7 @@
         <v>39</v>
       </c>
       <c r="B22" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
@@ -4394,7 +4391,7 @@
         <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
@@ -4402,7 +4399,7 @@
         <v>51</v>
       </c>
       <c r="B24" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
@@ -4410,7 +4407,7 @@
         <v>55</v>
       </c>
       <c r="B25" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
@@ -4418,7 +4415,7 @@
         <v>58</v>
       </c>
       <c r="B26" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
@@ -4426,7 +4423,7 @@
         <v>61</v>
       </c>
       <c r="B27" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
@@ -4434,7 +4431,7 @@
         <v>64</v>
       </c>
       <c r="B28" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
@@ -4442,7 +4439,7 @@
         <v>66</v>
       </c>
       <c r="B29" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
@@ -4450,7 +4447,7 @@
         <v>68</v>
       </c>
       <c r="B30" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
@@ -4458,7 +4455,7 @@
         <v>71</v>
       </c>
       <c r="B31" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
@@ -4466,7 +4463,7 @@
         <v>74</v>
       </c>
       <c r="B32" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
@@ -4474,7 +4471,7 @@
         <v>124</v>
       </c>
       <c r="B33" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
@@ -4482,7 +4479,7 @@
         <v>165</v>
       </c>
       <c r="B34" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
@@ -4490,7 +4487,7 @@
         <v>75</v>
       </c>
       <c r="B35" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
@@ -4498,7 +4495,7 @@
         <v>78</v>
       </c>
       <c r="B36" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
@@ -4506,15 +4503,15 @@
         <v>81</v>
       </c>
       <c r="B37" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
@@ -4522,7 +4519,7 @@
         <v>87</v>
       </c>
       <c r="B39" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
@@ -4530,7 +4527,7 @@
         <v>90</v>
       </c>
       <c r="B40" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
@@ -4538,7 +4535,7 @@
         <v>93</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
@@ -4546,7 +4543,7 @@
         <v>96</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
@@ -4554,7 +4551,7 @@
         <v>99</v>
       </c>
       <c r="B43" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
@@ -4562,7 +4559,7 @@
         <v>102</v>
       </c>
       <c r="B44" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
@@ -4570,7 +4567,7 @@
         <v>105</v>
       </c>
       <c r="B45" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
@@ -4578,15 +4575,15 @@
         <v>108</v>
       </c>
       <c r="B46" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
       <c r="B47" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
@@ -4594,7 +4591,7 @@
         <v>115</v>
       </c>
       <c r="B48" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.35">
@@ -4602,7 +4599,7 @@
         <v>118</v>
       </c>
       <c r="B49" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.35">
@@ -4610,175 +4607,175 @@
         <v>121</v>
       </c>
       <c r="B50" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A51" s="7" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="B51" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="B52" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="B53" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C53" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D53" t="s">
+        <v>260</v>
+      </c>
+      <c r="E53" t="s">
+        <v>260</v>
+      </c>
+      <c r="F53" t="s">
+        <v>260</v>
+      </c>
+      <c r="G53" t="s">
+        <v>260</v>
+      </c>
+      <c r="H53" t="s">
+        <v>260</v>
+      </c>
+      <c r="I53" t="s">
+        <v>260</v>
+      </c>
+      <c r="J53" t="s">
+        <v>260</v>
+      </c>
+      <c r="K53" t="s">
+        <v>260</v>
+      </c>
+      <c r="L53" t="s">
+        <v>261</v>
+      </c>
+      <c r="M53" t="s">
+        <v>260</v>
+      </c>
+      <c r="N53" t="s">
         <v>265</v>
-      </c>
-      <c r="E53" t="s">
-        <v>265</v>
-      </c>
-      <c r="F53" t="s">
-        <v>265</v>
-      </c>
-      <c r="G53" t="s">
-        <v>265</v>
-      </c>
-      <c r="H53" t="s">
-        <v>265</v>
-      </c>
-      <c r="I53" t="s">
-        <v>265</v>
-      </c>
-      <c r="J53" t="s">
-        <v>265</v>
-      </c>
-      <c r="K53" t="s">
-        <v>265</v>
-      </c>
-      <c r="L53" t="s">
-        <v>266</v>
-      </c>
-      <c r="M53" t="s">
-        <v>265</v>
-      </c>
-      <c r="N53" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="B54" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C54" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D54" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="E54" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="B55" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="B56" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="B57" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A58" s="8" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="B58" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C58" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="B59" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C59" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D59" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="B60" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C60" t="s">
+        <v>260</v>
+      </c>
+      <c r="D60" t="s">
+        <v>260</v>
+      </c>
+      <c r="E60" t="s">
         <v>265</v>
-      </c>
-      <c r="D60" t="s">
-        <v>265</v>
-      </c>
-      <c r="E60" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="B61" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C61" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D61" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="E61" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A62" s="7" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="B62" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -4799,7 +4796,7 @@
   </sheetPr>
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -4814,16 +4811,16 @@
         <v>173</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
@@ -4831,40 +4828,40 @@
         <v>129</v>
       </c>
       <c r="B2" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C2" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="D2" t="s">
+        <v>276</v>
+      </c>
+      <c r="E2" t="s">
+        <v>276</v>
+      </c>
+      <c r="F2" t="s">
+        <v>276</v>
+      </c>
+      <c r="G2" t="s">
+        <v>276</v>
+      </c>
+      <c r="H2" t="s">
+        <v>264</v>
+      </c>
+      <c r="I2" t="s">
+        <v>264</v>
+      </c>
+      <c r="J2" t="s">
+        <v>280</v>
+      </c>
+      <c r="K2" t="s">
         <v>281</v>
       </c>
-      <c r="E2" t="s">
-        <v>281</v>
-      </c>
-      <c r="F2" t="s">
-        <v>281</v>
-      </c>
-      <c r="G2" t="s">
-        <v>281</v>
-      </c>
-      <c r="H2" t="s">
-        <v>269</v>
-      </c>
-      <c r="I2" t="s">
-        <v>269</v>
-      </c>
-      <c r="J2" t="s">
-        <v>285</v>
-      </c>
-      <c r="K2" t="s">
-        <v>286</v>
-      </c>
       <c r="L2" s="13" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="N2" s="13"/>
     </row>
@@ -4873,34 +4870,34 @@
         <v>135</v>
       </c>
       <c r="B3" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C3" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="D3" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="E3" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="F3" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="G3" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="H3" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="I3" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
@@ -4908,34 +4905,34 @@
         <v>126</v>
       </c>
       <c r="B4" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C4" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="D4" t="s">
+        <v>276</v>
+      </c>
+      <c r="E4" t="s">
+        <v>276</v>
+      </c>
+      <c r="F4" t="s">
+        <v>282</v>
+      </c>
+      <c r="G4" t="s">
+        <v>282</v>
+      </c>
+      <c r="H4" t="s">
+        <v>280</v>
+      </c>
+      <c r="I4" t="s">
         <v>281</v>
       </c>
-      <c r="E4" t="s">
-        <v>281</v>
-      </c>
-      <c r="F4" t="s">
-        <v>287</v>
-      </c>
-      <c r="G4" t="s">
-        <v>287</v>
-      </c>
-      <c r="H4" t="s">
-        <v>285</v>
-      </c>
-      <c r="I4" t="s">
-        <v>286</v>
-      </c>
       <c r="J4" s="13" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
@@ -4943,34 +4940,34 @@
         <v>132</v>
       </c>
       <c r="B5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="D5" t="s">
+        <v>276</v>
+      </c>
+      <c r="E5" t="s">
+        <v>276</v>
+      </c>
+      <c r="F5" t="s">
+        <v>282</v>
+      </c>
+      <c r="G5" t="s">
+        <v>282</v>
+      </c>
+      <c r="H5" t="s">
+        <v>280</v>
+      </c>
+      <c r="I5" t="s">
         <v>281</v>
       </c>
-      <c r="E5" t="s">
-        <v>281</v>
-      </c>
-      <c r="F5" t="s">
-        <v>287</v>
-      </c>
-      <c r="G5" t="s">
-        <v>287</v>
-      </c>
-      <c r="H5" t="s">
-        <v>285</v>
-      </c>
-      <c r="I5" t="s">
-        <v>286</v>
-      </c>
       <c r="J5" s="13" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
@@ -4978,31 +4975,31 @@
         <v>138</v>
       </c>
       <c r="B6" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C6" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="D6" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="E6" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="F6" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="G6" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="H6" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -5010,10 +5007,10 @@
         <v>147</v>
       </c>
       <c r="B7" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="C7" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
@@ -5021,34 +5018,34 @@
         <v>141</v>
       </c>
       <c r="B8" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C8" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="D8" t="s">
+        <v>276</v>
+      </c>
+      <c r="E8" t="s">
+        <v>276</v>
+      </c>
+      <c r="F8" t="s">
+        <v>264</v>
+      </c>
+      <c r="G8" t="s">
+        <v>264</v>
+      </c>
+      <c r="H8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I8" t="s">
         <v>281</v>
       </c>
-      <c r="E8" t="s">
-        <v>281</v>
-      </c>
-      <c r="F8" t="s">
-        <v>269</v>
-      </c>
-      <c r="G8" t="s">
-        <v>269</v>
-      </c>
-      <c r="H8" t="s">
-        <v>285</v>
-      </c>
-      <c r="I8" t="s">
-        <v>286</v>
-      </c>
       <c r="J8" s="13" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
@@ -5056,100 +5053,100 @@
         <v>144</v>
       </c>
       <c r="B9" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C9" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="D9" t="s">
+        <v>276</v>
+      </c>
+      <c r="E9" t="s">
+        <v>276</v>
+      </c>
+      <c r="F9" t="s">
+        <v>264</v>
+      </c>
+      <c r="G9" t="s">
+        <v>264</v>
+      </c>
+      <c r="H9" t="s">
+        <v>280</v>
+      </c>
+      <c r="I9" t="s">
         <v>281</v>
       </c>
-      <c r="E9" t="s">
-        <v>281</v>
-      </c>
-      <c r="F9" t="s">
-        <v>269</v>
-      </c>
-      <c r="G9" t="s">
-        <v>269</v>
-      </c>
-      <c r="H9" t="s">
-        <v>285</v>
-      </c>
-      <c r="I9" t="s">
-        <v>286</v>
-      </c>
       <c r="J9" s="13" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="K9" s="13" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="B10" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="C10" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="B11" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="C11" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D11" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="E11" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="F11" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="B12" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C12" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D12" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="E12" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="F12" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="G12" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="H12" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="I12" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="J12" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="K12" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
@@ -5157,7 +5154,7 @@
         <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
@@ -5165,7 +5162,7 @@
         <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
@@ -5173,13 +5170,13 @@
         <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="C15" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D15" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
@@ -5187,7 +5184,7 @@
         <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -5195,7 +5192,7 @@
         <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -5203,7 +5200,7 @@
         <v>61</v>
       </c>
       <c r="B18" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -5211,7 +5208,7 @@
         <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -5219,7 +5216,7 @@
         <v>66</v>
       </c>
       <c r="B20" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -5227,7 +5224,7 @@
         <v>68</v>
       </c>
       <c r="B21" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -5235,7 +5232,7 @@
         <v>74</v>
       </c>
       <c r="B22" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -5243,7 +5240,7 @@
         <v>124</v>
       </c>
       <c r="B23" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -5251,7 +5248,7 @@
         <v>75</v>
       </c>
       <c r="B24" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -5259,7 +5256,7 @@
         <v>78</v>
       </c>
       <c r="B25" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
@@ -5267,7 +5264,7 @@
         <v>87</v>
       </c>
       <c r="B26" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
@@ -5275,7 +5272,7 @@
         <v>90</v>
       </c>
       <c r="B27" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
@@ -5283,7 +5280,7 @@
         <v>93</v>
       </c>
       <c r="B28" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
@@ -5291,7 +5288,7 @@
         <v>96</v>
       </c>
       <c r="B29" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
@@ -5299,7 +5296,7 @@
         <v>99</v>
       </c>
       <c r="B30" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
@@ -5307,7 +5304,7 @@
         <v>102</v>
       </c>
       <c r="B31" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -5315,7 +5312,7 @@
         <v>105</v>
       </c>
       <c r="B32" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.35">
@@ -5323,7 +5320,7 @@
         <v>108</v>
       </c>
       <c r="B33" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.35">
@@ -5331,7 +5328,7 @@
         <v>115</v>
       </c>
       <c r="B34" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.35">
@@ -5339,7 +5336,7 @@
         <v>118</v>
       </c>
       <c r="B35" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.35">
@@ -5347,135 +5344,135 @@
         <v>121</v>
       </c>
       <c r="B36" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37" s="7" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="B37" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="B38" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C38" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="D38" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="E38" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="F38" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="G38" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="H38" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="I38" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="J38" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="K38" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="L38" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="M38" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="N38" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="B39" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C39" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="D39" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="E39" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A40" s="8" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="B40" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C40" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="B41" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C41" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D41" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="B42" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C42" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="D42" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="E42" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="B43" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C43" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="D43" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="E43" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -5497,9 +5494,9 @@
   <dimension ref="A1:W54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A34" sqref="A34"/>
-      <selection pane="topRight" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5533,31 +5530,31 @@
         <v>173</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>291</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>293</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>294</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
@@ -5565,43 +5562,43 @@
         <v>129</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="E2" t="s">
+        <v>352</v>
+      </c>
+      <c r="F2" t="s">
+        <v>353</v>
+      </c>
+      <c r="G2" t="s">
+        <v>354</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>355</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="J2" s="13" t="s">
         <v>357</v>
       </c>
-      <c r="F2" t="s">
+      <c r="K2" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="M2" s="13" t="s">
         <v>358</v>
       </c>
-      <c r="G2" t="s">
-        <v>359</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>360</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>361</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>362</v>
-      </c>
-      <c r="K2" s="13" t="s">
+      <c r="N2" s="13" t="s">
         <v>351</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>352</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>363</v>
-      </c>
-      <c r="N2" s="13" t="s">
-        <v>356</v>
       </c>
       <c r="O2" s="13"/>
       <c r="P2" s="13"/>
@@ -5612,22 +5609,22 @@
         <v>150</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>426</v>
+        <v>466</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>371</v>
+        <v>343</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
@@ -5635,22 +5632,22 @@
         <v>153</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>426</v>
+        <v>466</v>
       </c>
       <c r="C4" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="D4" t="s">
+        <v>370</v>
+      </c>
+      <c r="E4" s="13" t="s">
         <v>371</v>
       </c>
-      <c r="D4" t="s">
-        <v>376</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>377</v>
-      </c>
       <c r="F4" s="13" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
@@ -5658,37 +5655,37 @@
         <v>135</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="C5" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="E5" s="13" t="s">
         <v>348</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>349</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>353</v>
-      </c>
       <c r="F5" s="13" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="L5" s="13" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
@@ -5696,37 +5693,37 @@
         <v>126</v>
       </c>
       <c r="B6" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="C6" t="s">
+        <v>343</v>
+      </c>
+      <c r="D6" t="s">
+        <v>344</v>
+      </c>
+      <c r="E6" t="s">
         <v>348</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>349</v>
       </c>
-      <c r="E6" t="s">
-        <v>353</v>
-      </c>
-      <c r="F6" t="s">
-        <v>354</v>
-      </c>
       <c r="G6" s="13" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="H6" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="I6" t="s">
+        <v>346</v>
+      </c>
+      <c r="J6" t="s">
+        <v>347</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>462</v>
+      </c>
+      <c r="L6" s="13" t="s">
         <v>351</v>
-      </c>
-      <c r="J6" t="s">
-        <v>352</v>
-      </c>
-      <c r="K6" s="13" t="s">
-        <v>469</v>
-      </c>
-      <c r="L6" s="13" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
@@ -5734,37 +5731,37 @@
         <v>132</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="C7" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="E7" s="13" t="s">
         <v>348</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="F7" s="13" t="s">
         <v>349</v>
       </c>
-      <c r="E7" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>354</v>
-      </c>
       <c r="G7" s="13" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="I7" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>462</v>
+      </c>
+      <c r="L7" s="13" t="s">
         <v>351</v>
-      </c>
-      <c r="J7" s="13" t="s">
-        <v>352</v>
-      </c>
-      <c r="K7" s="13" t="s">
-        <v>469</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>356</v>
       </c>
       <c r="M7" s="13"/>
       <c r="N7" s="13"/>
@@ -5774,34 +5771,34 @@
         <v>138</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="C8" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="E8" s="13" t="s">
         <v>348</v>
       </c>
-      <c r="D8" s="13" t="s">
-        <v>349</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>353</v>
-      </c>
       <c r="F8" s="13" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="I8" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>462</v>
+      </c>
+      <c r="K8" s="13" t="s">
         <v>351</v>
-      </c>
-      <c r="J8" s="13" t="s">
-        <v>469</v>
-      </c>
-      <c r="K8" s="13" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.35">
@@ -5809,13 +5806,13 @@
         <v>147</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="D9" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.35">
@@ -5823,37 +5820,37 @@
         <v>141</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="C10" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="E10" s="13" t="s">
         <v>348</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="F10" s="13" t="s">
         <v>349</v>
       </c>
-      <c r="E10" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>354</v>
-      </c>
       <c r="G10" s="13" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="I10" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="J10" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="K10" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="L10" s="13" t="s">
         <v>351</v>
-      </c>
-      <c r="J10" s="13" t="s">
-        <v>352</v>
-      </c>
-      <c r="K10" s="13" t="s">
-        <v>363</v>
-      </c>
-      <c r="L10" s="13" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.35">
@@ -5861,247 +5858,247 @@
         <v>144</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="C11" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="E11" s="13" t="s">
         <v>348</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="F11" s="13" t="s">
         <v>349</v>
       </c>
-      <c r="E11" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>354</v>
-      </c>
       <c r="G11" s="13" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="I11" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="L11" s="13" t="s">
         <v>351</v>
-      </c>
-      <c r="J11" s="13" t="s">
-        <v>352</v>
-      </c>
-      <c r="K11" s="13" t="s">
-        <v>363</v>
-      </c>
-      <c r="L11" s="13" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D12" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="C13" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="H13" s="6" t="s">
         <v>315</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>317</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>319</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="C14" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="H14" s="6" t="s">
         <v>315</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>317</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>319</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="C16" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="E16" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="F16" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="G16" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="C17" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="E17" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="F17" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="G17" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="C18" t="s">
+        <v>321</v>
+      </c>
+      <c r="D18" t="s">
         <v>326</v>
       </c>
-      <c r="D18" t="s">
-        <v>331</v>
-      </c>
       <c r="E18" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="C19" t="s">
+        <v>328</v>
+      </c>
+      <c r="D19" t="s">
+        <v>329</v>
+      </c>
+      <c r="E19" t="s">
+        <v>330</v>
+      </c>
+      <c r="F19" t="s">
+        <v>331</v>
+      </c>
+      <c r="G19" t="s">
+        <v>332</v>
+      </c>
+      <c r="H19" t="s">
         <v>333</v>
-      </c>
-      <c r="D19" t="s">
-        <v>334</v>
-      </c>
-      <c r="E19" t="s">
-        <v>335</v>
-      </c>
-      <c r="F19" t="s">
-        <v>336</v>
-      </c>
-      <c r="G19" t="s">
-        <v>337</v>
-      </c>
-      <c r="H19" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="C20" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>336</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="H20" s="12" t="s">
         <v>339</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="I20" s="12" t="s">
         <v>340</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="J20" s="12" t="s">
         <v>341</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="K20" s="12" t="s">
+        <v>299</v>
+      </c>
+      <c r="L20" s="12" t="s">
         <v>342</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>343</v>
-      </c>
-      <c r="H20" s="12" t="s">
-        <v>344</v>
-      </c>
-      <c r="I20" s="12" t="s">
-        <v>345</v>
-      </c>
-      <c r="J20" s="12" t="s">
-        <v>346</v>
-      </c>
-      <c r="K20" s="12" t="s">
-        <v>304</v>
-      </c>
-      <c r="L20" s="12" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.35">
@@ -6109,10 +6106,10 @@
         <v>32</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="C21" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
@@ -6120,10 +6117,10 @@
         <v>36</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="C22" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.35">
@@ -6131,10 +6128,10 @@
         <v>39</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="C23" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.35">
@@ -6142,10 +6139,10 @@
         <v>42</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="C24" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.35">
@@ -6153,10 +6150,10 @@
         <v>48</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="C25" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.35">
@@ -6164,10 +6161,10 @@
         <v>51</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="C26" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.35">
@@ -6175,10 +6172,10 @@
         <v>55</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="C27" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.35">
@@ -6186,10 +6183,10 @@
         <v>58</v>
       </c>
       <c r="B28" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="C28" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.35">
@@ -6197,10 +6194,10 @@
         <v>61</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="C29" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.35">
@@ -6208,10 +6205,10 @@
         <v>64</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="C30" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.35">
@@ -6219,10 +6216,10 @@
         <v>66</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="C31" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.35">
@@ -6230,10 +6227,10 @@
         <v>68</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="C32" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.35">
@@ -6241,10 +6238,10 @@
         <v>71</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="C33" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.35">
@@ -6252,10 +6249,10 @@
         <v>74</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="C34" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.35">
@@ -6263,10 +6260,10 @@
         <v>124</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="C35" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.35">
@@ -6274,10 +6271,10 @@
         <v>165</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="C36" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.35">
@@ -6285,10 +6282,10 @@
         <v>75</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="C37" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.35">
@@ -6296,10 +6293,10 @@
         <v>78</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="C38" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.35">
@@ -6307,21 +6304,21 @@
         <v>81</v>
       </c>
       <c r="B39" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="C39" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
     </row>
     <row r="40" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="B40" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="C40" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="D40"/>
       <c r="E40"/>
@@ -6343,10 +6340,10 @@
         <v>87</v>
       </c>
       <c r="B41" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="C41" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.35">
@@ -6354,10 +6351,10 @@
         <v>90</v>
       </c>
       <c r="B42" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="C42" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.35">
@@ -6365,10 +6362,10 @@
         <v>93</v>
       </c>
       <c r="B43" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="C43" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.35">
@@ -6376,10 +6373,10 @@
         <v>96</v>
       </c>
       <c r="B44" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="C44" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.35">
@@ -6387,10 +6384,10 @@
         <v>99</v>
       </c>
       <c r="B45" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="C45" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.35">
@@ -6398,10 +6395,10 @@
         <v>102</v>
       </c>
       <c r="B46" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="C46" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.35">
@@ -6409,10 +6406,10 @@
         <v>105</v>
       </c>
       <c r="B47" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="C47" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.35">
@@ -6420,21 +6417,21 @@
         <v>108</v>
       </c>
       <c r="B48" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="C48" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
       <c r="B49" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="C49" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="U49" s="13"/>
       <c r="V49" s="13"/>
@@ -6532,22 +6529,22 @@
         <v>173</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -6555,10 +6552,10 @@
         <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="C2" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -6566,10 +6563,10 @@
         <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="C3" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -6577,10 +6574,10 @@
         <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="C4" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -6588,22 +6585,22 @@
         <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="C5" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="D5" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="E5" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="F5" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="G5" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Identify rated voltage as the "U" phase voltage in the electrical module. Identify thickness as the wall thickness of a pile in the moorings module.
</commit_message>
<xml_diff>
--- a/dds/moorings.xlsx
+++ b/dds/moorings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="419" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1258" uniqueCount="474">
   <si>
     <t>Identifier</t>
   </si>
@@ -731,9 +731,6 @@
     <t>Youngs Modulus</t>
   </si>
   <si>
-    <t>Thickness</t>
-  </si>
-  <si>
     <t>Extension</t>
   </si>
   <si>
@@ -1121,9 +1118,6 @@
     <t>youngs_modulus</t>
   </si>
   <si>
-    <t>thickness</t>
-  </si>
-  <si>
     <t>maximum_displacement</t>
   </si>
   <si>
@@ -1452,6 +1446,18 @@
   </si>
   <si>
     <t>reference.view_soil_type_geotechnical_properties</t>
+  </si>
+  <si>
+    <t>Nominal Diameter</t>
+  </si>
+  <si>
+    <t>nominal_diameter</t>
+  </si>
+  <si>
+    <t>wall_thickness</t>
+  </si>
+  <si>
+    <t>Wall Thickness</t>
   </si>
 </sst>
 </file>
@@ -2034,10 +2040,10 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
@@ -2149,7 +2155,7 @@
         <v>147</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>148</v>
@@ -2192,7 +2198,7 @@
     </row>
     <row r="12" spans="1:8" s="15" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="15" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>6</v>
@@ -2206,7 +2212,7 @@
     </row>
     <row r="13" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>9</v>
@@ -2220,7 +2226,7 @@
     </row>
     <row r="14" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>9</v>
@@ -2234,7 +2240,7 @@
     </row>
     <row r="15" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>9</v>
@@ -2248,7 +2254,7 @@
     </row>
     <row r="16" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="15" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>9</v>
@@ -2266,7 +2272,7 @@
     </row>
     <row r="17" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="15" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>9</v>
@@ -2280,7 +2286,7 @@
     </row>
     <row r="18" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="15" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>9</v>
@@ -2294,7 +2300,7 @@
     </row>
     <row r="19" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="15" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>9</v>
@@ -2308,7 +2314,7 @@
     </row>
     <row r="20" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="15" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B20" s="15" t="s">
         <v>26</v>
@@ -2484,7 +2490,7 @@
         <v>65</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
@@ -2504,7 +2510,7 @@
         <v>67</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G31" s="15" t="s">
         <v>33</v>
@@ -2541,7 +2547,7 @@
         <v>73</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="G33" s="15" t="s">
         <v>33</v>
@@ -2555,10 +2561,10 @@
         <v>24</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="G34" s="15" t="s">
         <v>33</v>
@@ -2575,7 +2581,7 @@
         <v>125</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="G35" s="15" t="s">
         <v>33</v>
@@ -2654,16 +2660,16 @@
     </row>
     <row r="40" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="16" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B40" s="15" t="s">
         <v>24</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="E40" s="15"/>
       <c r="F40" s="15"/>
@@ -2820,7 +2826,7 @@
     </row>
     <row r="49" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="17" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B49" s="15" t="s">
         <v>24</v>
@@ -2829,7 +2835,7 @@
         <v>25</v>
       </c>
       <c r="D49" s="18" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="50" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
@@ -2884,13 +2890,13 @@
     </row>
     <row r="53" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="20" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B53" s="14" t="s">
         <v>24</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D53" s="14" t="s">
         <v>29</v>
@@ -2902,7 +2908,7 @@
     </row>
     <row r="54" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="14" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B54" s="14" t="s">
         <v>24</v>
@@ -2922,7 +2928,7 @@
     </row>
     <row r="55" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>159</v>
@@ -2942,7 +2948,7 @@
     </row>
     <row r="56" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>159</v>
@@ -2957,7 +2963,7 @@
     </row>
     <row r="57" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A57" s="19" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B57" s="14" t="s">
         <v>28</v>
@@ -2975,7 +2981,7 @@
     </row>
     <row r="58" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="19" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B58" s="14" t="s">
         <v>28</v>
@@ -2993,7 +2999,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" s="19" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B59" s="14" t="s">
         <v>28</v>
@@ -3011,7 +3017,7 @@
     </row>
     <row r="60" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>159</v>
@@ -3029,13 +3035,13 @@
     </row>
     <row r="61" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>159</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>172</v>
@@ -3047,13 +3053,13 @@
     </row>
     <row r="62" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>159</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>160</v>
@@ -3064,13 +3070,13 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>156</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>157</v>
@@ -3084,7 +3090,7 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>159</v>
@@ -3101,13 +3107,13 @@
     </row>
     <row r="65" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A65" s="19" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B65" s="14" t="s">
         <v>30</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D65" s="14" t="s">
         <v>31</v>
@@ -3135,9 +3141,9 @@
   </sheetPr>
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3221,7 +3227,7 @@
         <v>228</v>
       </c>
       <c r="J2" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="K2" t="s">
         <v>216</v>
@@ -3242,16 +3248,16 @@
         <v>213</v>
       </c>
       <c r="C3" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>233</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="E3" t="s">
         <v>234</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>235</v>
-      </c>
-      <c r="F3" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
@@ -3262,16 +3268,16 @@
         <v>213</v>
       </c>
       <c r="C4" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>233</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="E4" t="s">
         <v>234</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>235</v>
-      </c>
-      <c r="F4" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
@@ -3288,7 +3294,7 @@
         <v>217</v>
       </c>
       <c r="E5" t="s">
-        <v>231</v>
+        <v>473</v>
       </c>
       <c r="F5" t="s">
         <v>219</v>
@@ -3303,7 +3309,7 @@
         <v>230</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="K5" s="13" t="s">
         <v>222</v>
@@ -3332,13 +3338,13 @@
         <v>220</v>
       </c>
       <c r="H6" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="I6" t="s">
         <v>216</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="K6" s="13" t="s">
         <v>222</v>
@@ -3367,13 +3373,13 @@
         <v>220</v>
       </c>
       <c r="H7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="I7" t="s">
         <v>216</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="K7" s="13" t="s">
         <v>222</v>
@@ -3402,10 +3408,10 @@
         <v>215</v>
       </c>
       <c r="H8" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="J8" s="13" t="s">
         <v>222</v>
@@ -3419,10 +3425,10 @@
         <v>213</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.35">
@@ -3436,27 +3442,36 @@
         <v>214</v>
       </c>
       <c r="D10" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="E10" t="s">
+        <v>224</v>
+      </c>
+      <c r="F10" t="s">
+        <v>225</v>
+      </c>
+      <c r="G10" t="s">
+        <v>470</v>
+      </c>
+      <c r="H10" t="s">
         <v>218</v>
       </c>
-      <c r="F10" t="s">
+      <c r="I10" t="s">
         <v>227</v>
       </c>
-      <c r="G10" t="s">
+      <c r="J10" t="s">
         <v>228</v>
       </c>
-      <c r="H10" t="s">
-        <v>469</v>
-      </c>
-      <c r="I10" t="s">
+      <c r="K10" t="s">
+        <v>467</v>
+      </c>
+      <c r="L10" t="s">
         <v>216</v>
       </c>
-      <c r="J10" s="13" t="s">
+      <c r="M10" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="K10" s="8" t="s">
+      <c r="N10" s="13" t="s">
         <v>222</v>
       </c>
     </row>
@@ -3471,33 +3486,42 @@
         <v>214</v>
       </c>
       <c r="D11" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="E11" t="s">
+        <v>224</v>
+      </c>
+      <c r="F11" t="s">
+        <v>225</v>
+      </c>
+      <c r="G11" t="s">
+        <v>470</v>
+      </c>
+      <c r="H11" t="s">
         <v>218</v>
       </c>
-      <c r="F11" t="s">
+      <c r="I11" t="s">
         <v>227</v>
       </c>
-      <c r="G11" t="s">
+      <c r="J11" t="s">
         <v>228</v>
       </c>
-      <c r="H11" t="s">
-        <v>469</v>
-      </c>
-      <c r="I11" t="s">
+      <c r="K11" t="s">
+        <v>467</v>
+      </c>
+      <c r="L11" t="s">
         <v>216</v>
       </c>
-      <c r="J11" s="13" t="s">
+      <c r="M11" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="K11" s="13" t="s">
+      <c r="N11" s="13" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B12" t="s">
         <v>180</v>
@@ -3508,7 +3532,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>182</v>
@@ -3540,7 +3564,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B14" t="s">
         <v>182</v>
@@ -3563,7 +3587,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B15" t="s">
         <v>182</v>
@@ -3577,7 +3601,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B16" t="s">
         <v>180</v>
@@ -3586,18 +3610,18 @@
         <v>190</v>
       </c>
       <c r="D16" t="s">
+        <v>464</v>
+      </c>
+      <c r="E16" t="s">
+        <v>465</v>
+      </c>
+      <c r="F16" t="s">
         <v>466</v>
-      </c>
-      <c r="E16" t="s">
-        <v>467</v>
-      </c>
-      <c r="F16" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B17" t="s">
         <v>191</v>
@@ -3617,7 +3641,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B18" t="s">
         <v>191</v>
@@ -3631,7 +3655,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B19" t="s">
         <v>198</v>
@@ -3654,7 +3678,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B20" t="s">
         <v>204</v>
@@ -3689,25 +3713,25 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B21" t="s">
+        <v>238</v>
+      </c>
+      <c r="C21" t="s">
         <v>239</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>240</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>241</v>
-      </c>
-      <c r="E21" t="s">
-        <v>242</v>
       </c>
       <c r="F21" t="s">
         <v>224</v>
       </c>
       <c r="G21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H21" t="s">
         <v>223</v>
@@ -3716,27 +3740,27 @@
         <v>225</v>
       </c>
       <c r="J21" t="s">
+        <v>243</v>
+      </c>
+      <c r="K21" t="s">
         <v>244</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>245</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
         <v>246</v>
       </c>
-      <c r="M21" t="s">
+      <c r="N21" t="s">
         <v>247</v>
-      </c>
-      <c r="N21" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C22" t="s">
         <v>204</v>
@@ -3745,37 +3769,37 @@
         <v>224</v>
       </c>
       <c r="E22" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B23" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C23" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B24" t="s">
+        <v>250</v>
+      </c>
+      <c r="C24" t="s">
         <v>251</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>252</v>
-      </c>
-      <c r="D24" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B25" t="s">
         <v>213</v>
@@ -3784,27 +3808,27 @@
         <v>221</v>
       </c>
       <c r="D25" t="s">
+        <v>236</v>
+      </c>
+      <c r="E25" t="s">
         <v>237</v>
-      </c>
-      <c r="E25" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B26" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C26" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D26" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E26" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -3826,7 +3850,7 @@
   <dimension ref="A1:U62"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B10" sqref="B10:N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3840,22 +3864,22 @@
         <v>173</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>257</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>258</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.35">
@@ -3863,40 +3887,40 @@
         <v>129</v>
       </c>
       <c r="B2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D2" t="s">
+        <v>259</v>
+      </c>
+      <c r="E2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F2" t="s">
+        <v>259</v>
+      </c>
+      <c r="G2" t="s">
+        <v>259</v>
+      </c>
+      <c r="H2" t="s">
+        <v>259</v>
+      </c>
+      <c r="I2" t="s">
+        <v>259</v>
+      </c>
+      <c r="J2" t="s">
+        <v>259</v>
+      </c>
+      <c r="K2" t="s">
+        <v>259</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="M2" s="13" t="s">
         <v>260</v>
-      </c>
-      <c r="E2" t="s">
-        <v>260</v>
-      </c>
-      <c r="F2" t="s">
-        <v>260</v>
-      </c>
-      <c r="G2" t="s">
-        <v>260</v>
-      </c>
-      <c r="H2" t="s">
-        <v>260</v>
-      </c>
-      <c r="I2" t="s">
-        <v>260</v>
-      </c>
-      <c r="J2" t="s">
-        <v>260</v>
-      </c>
-      <c r="K2" t="s">
-        <v>260</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>260</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>261</v>
       </c>
       <c r="O2" s="13"/>
       <c r="P2" s="13"/>
@@ -3907,19 +3931,19 @@
         <v>150</v>
       </c>
       <c r="B3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
@@ -3927,19 +3951,19 @@
         <v>153</v>
       </c>
       <c r="B4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.35">
@@ -3947,34 +3971,34 @@
         <v>135</v>
       </c>
       <c r="B5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D5" t="s">
+        <v>259</v>
+      </c>
+      <c r="E5" t="s">
+        <v>259</v>
+      </c>
+      <c r="F5" t="s">
+        <v>259</v>
+      </c>
+      <c r="G5" t="s">
+        <v>259</v>
+      </c>
+      <c r="H5" t="s">
+        <v>259</v>
+      </c>
+      <c r="I5" t="s">
+        <v>259</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="K5" s="13" t="s">
         <v>260</v>
-      </c>
-      <c r="E5" t="s">
-        <v>260</v>
-      </c>
-      <c r="F5" t="s">
-        <v>260</v>
-      </c>
-      <c r="G5" t="s">
-        <v>260</v>
-      </c>
-      <c r="H5" t="s">
-        <v>260</v>
-      </c>
-      <c r="I5" t="s">
-        <v>260</v>
-      </c>
-      <c r="J5" s="13" t="s">
-        <v>260</v>
-      </c>
-      <c r="K5" s="13" t="s">
-        <v>261</v>
       </c>
       <c r="M5" s="13"/>
       <c r="N5" s="13"/>
@@ -3984,34 +4008,34 @@
         <v>126</v>
       </c>
       <c r="B6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D6" t="s">
+        <v>259</v>
+      </c>
+      <c r="E6" t="s">
+        <v>259</v>
+      </c>
+      <c r="F6" t="s">
+        <v>259</v>
+      </c>
+      <c r="G6" t="s">
+        <v>259</v>
+      </c>
+      <c r="H6" t="s">
+        <v>259</v>
+      </c>
+      <c r="I6" t="s">
+        <v>259</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="K6" s="13" t="s">
         <v>260</v>
-      </c>
-      <c r="E6" t="s">
-        <v>260</v>
-      </c>
-      <c r="F6" t="s">
-        <v>260</v>
-      </c>
-      <c r="G6" t="s">
-        <v>260</v>
-      </c>
-      <c r="H6" t="s">
-        <v>260</v>
-      </c>
-      <c r="I6" t="s">
-        <v>260</v>
-      </c>
-      <c r="J6" s="13" t="s">
-        <v>260</v>
-      </c>
-      <c r="K6" s="13" t="s">
-        <v>261</v>
       </c>
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
@@ -4021,34 +4045,34 @@
         <v>132</v>
       </c>
       <c r="B7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D7" t="s">
+        <v>259</v>
+      </c>
+      <c r="E7" t="s">
+        <v>259</v>
+      </c>
+      <c r="F7" t="s">
+        <v>259</v>
+      </c>
+      <c r="G7" t="s">
+        <v>259</v>
+      </c>
+      <c r="H7" t="s">
+        <v>259</v>
+      </c>
+      <c r="I7" t="s">
+        <v>259</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="K7" s="13" t="s">
         <v>260</v>
-      </c>
-      <c r="E7" t="s">
-        <v>260</v>
-      </c>
-      <c r="F7" t="s">
-        <v>260</v>
-      </c>
-      <c r="G7" t="s">
-        <v>260</v>
-      </c>
-      <c r="H7" t="s">
-        <v>260</v>
-      </c>
-      <c r="I7" t="s">
-        <v>260</v>
-      </c>
-      <c r="J7" s="13" t="s">
-        <v>260</v>
-      </c>
-      <c r="K7" s="13" t="s">
-        <v>261</v>
       </c>
       <c r="M7" s="13"/>
       <c r="N7" s="13"/>
@@ -4058,31 +4082,31 @@
         <v>138</v>
       </c>
       <c r="B8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D8" t="s">
+        <v>259</v>
+      </c>
+      <c r="E8" t="s">
+        <v>259</v>
+      </c>
+      <c r="F8" t="s">
+        <v>259</v>
+      </c>
+      <c r="G8" t="s">
         <v>260</v>
       </c>
-      <c r="E8" t="s">
+      <c r="H8" t="s">
+        <v>259</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="J8" s="13" t="s">
         <v>260</v>
-      </c>
-      <c r="F8" t="s">
-        <v>260</v>
-      </c>
-      <c r="G8" t="s">
-        <v>261</v>
-      </c>
-      <c r="H8" t="s">
-        <v>260</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>260</v>
-      </c>
-      <c r="J8" s="13" t="s">
-        <v>261</v>
       </c>
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
@@ -4092,84 +4116,98 @@
         <v>141</v>
       </c>
       <c r="B9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D9" t="s">
+        <v>259</v>
+      </c>
+      <c r="E9" t="s">
+        <v>259</v>
+      </c>
+      <c r="F9" t="s">
+        <v>259</v>
+      </c>
+      <c r="G9" t="s">
+        <v>259</v>
+      </c>
+      <c r="H9" t="s">
+        <v>259</v>
+      </c>
+      <c r="I9" t="s">
+        <v>259</v>
+      </c>
+      <c r="J9" t="s">
+        <v>259</v>
+      </c>
+      <c r="K9" t="s">
+        <v>259</v>
+      </c>
+      <c r="L9" t="s">
+        <v>259</v>
+      </c>
+      <c r="M9" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="N9" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="E9" t="s">
-        <v>260</v>
-      </c>
-      <c r="F9" t="s">
-        <v>260</v>
-      </c>
-      <c r="G9" t="s">
-        <v>260</v>
-      </c>
-      <c r="H9" t="s">
-        <v>260</v>
-      </c>
-      <c r="I9" t="s">
-        <v>260</v>
-      </c>
-      <c r="J9" s="13" t="s">
-        <v>260</v>
-      </c>
-      <c r="K9" s="13" t="s">
-        <v>261</v>
-      </c>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
         <v>144</v>
       </c>
       <c r="B10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D10" t="s">
+        <v>259</v>
+      </c>
+      <c r="E10" t="s">
+        <v>259</v>
+      </c>
+      <c r="F10" t="s">
+        <v>259</v>
+      </c>
+      <c r="G10" t="s">
+        <v>259</v>
+      </c>
+      <c r="H10" t="s">
+        <v>259</v>
+      </c>
+      <c r="I10" t="s">
+        <v>259</v>
+      </c>
+      <c r="J10" t="s">
+        <v>259</v>
+      </c>
+      <c r="K10" t="s">
+        <v>259</v>
+      </c>
+      <c r="L10" t="s">
+        <v>259</v>
+      </c>
+      <c r="M10" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="N10" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="E10" t="s">
-        <v>260</v>
-      </c>
-      <c r="F10" t="s">
-        <v>260</v>
-      </c>
-      <c r="G10" t="s">
-        <v>260</v>
-      </c>
-      <c r="H10" t="s">
-        <v>260</v>
-      </c>
-      <c r="I10" t="s">
-        <v>260</v>
-      </c>
-      <c r="J10" s="13" t="s">
-        <v>260</v>
-      </c>
-      <c r="K10" s="13" t="s">
-        <v>261</v>
-      </c>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -4192,174 +4230,174 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B16" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C16" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D16" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E16" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F16" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B17" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C17" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D17" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
@@ -4367,7 +4405,7 @@
         <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
@@ -4375,7 +4413,7 @@
         <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
@@ -4383,7 +4421,7 @@
         <v>39</v>
       </c>
       <c r="B22" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
@@ -4391,7 +4429,7 @@
         <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
@@ -4399,7 +4437,7 @@
         <v>51</v>
       </c>
       <c r="B24" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
@@ -4407,7 +4445,7 @@
         <v>55</v>
       </c>
       <c r="B25" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
@@ -4415,7 +4453,7 @@
         <v>58</v>
       </c>
       <c r="B26" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
@@ -4423,7 +4461,7 @@
         <v>61</v>
       </c>
       <c r="B27" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
@@ -4431,7 +4469,7 @@
         <v>64</v>
       </c>
       <c r="B28" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
@@ -4439,7 +4477,7 @@
         <v>66</v>
       </c>
       <c r="B29" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
@@ -4447,7 +4485,7 @@
         <v>68</v>
       </c>
       <c r="B30" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
@@ -4455,7 +4493,7 @@
         <v>71</v>
       </c>
       <c r="B31" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
@@ -4463,7 +4501,7 @@
         <v>74</v>
       </c>
       <c r="B32" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
@@ -4471,7 +4509,7 @@
         <v>124</v>
       </c>
       <c r="B33" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
@@ -4479,7 +4517,7 @@
         <v>165</v>
       </c>
       <c r="B34" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
@@ -4487,7 +4525,7 @@
         <v>75</v>
       </c>
       <c r="B35" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
@@ -4495,7 +4533,7 @@
         <v>78</v>
       </c>
       <c r="B36" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
@@ -4503,15 +4541,15 @@
         <v>81</v>
       </c>
       <c r="B37" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
@@ -4519,7 +4557,7 @@
         <v>87</v>
       </c>
       <c r="B39" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
@@ -4527,7 +4565,7 @@
         <v>90</v>
       </c>
       <c r="B40" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
@@ -4535,7 +4573,7 @@
         <v>93</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
@@ -4543,7 +4581,7 @@
         <v>96</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
@@ -4551,7 +4589,7 @@
         <v>99</v>
       </c>
       <c r="B43" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
@@ -4559,7 +4597,7 @@
         <v>102</v>
       </c>
       <c r="B44" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
@@ -4567,7 +4605,7 @@
         <v>105</v>
       </c>
       <c r="B45" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
@@ -4575,15 +4613,15 @@
         <v>108</v>
       </c>
       <c r="B46" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B47" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
@@ -4591,7 +4629,7 @@
         <v>115</v>
       </c>
       <c r="B48" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.35">
@@ -4599,7 +4637,7 @@
         <v>118</v>
       </c>
       <c r="B49" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.35">
@@ -4607,175 +4645,175 @@
         <v>121</v>
       </c>
       <c r="B50" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A51" s="7" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B51" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B52" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B53" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C53" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D53" t="s">
+        <v>259</v>
+      </c>
+      <c r="E53" t="s">
+        <v>259</v>
+      </c>
+      <c r="F53" t="s">
+        <v>259</v>
+      </c>
+      <c r="G53" t="s">
+        <v>259</v>
+      </c>
+      <c r="H53" t="s">
+        <v>259</v>
+      </c>
+      <c r="I53" t="s">
+        <v>259</v>
+      </c>
+      <c r="J53" t="s">
+        <v>259</v>
+      </c>
+      <c r="K53" t="s">
+        <v>259</v>
+      </c>
+      <c r="L53" t="s">
         <v>260</v>
       </c>
-      <c r="E53" t="s">
-        <v>260</v>
-      </c>
-      <c r="F53" t="s">
-        <v>260</v>
-      </c>
-      <c r="G53" t="s">
-        <v>260</v>
-      </c>
-      <c r="H53" t="s">
-        <v>260</v>
-      </c>
-      <c r="I53" t="s">
-        <v>260</v>
-      </c>
-      <c r="J53" t="s">
-        <v>260</v>
-      </c>
-      <c r="K53" t="s">
-        <v>260</v>
-      </c>
-      <c r="L53" t="s">
-        <v>261</v>
-      </c>
       <c r="M53" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="N53" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B54" t="s">
+        <v>259</v>
+      </c>
+      <c r="C54" t="s">
         <v>260</v>
       </c>
-      <c r="C54" t="s">
-        <v>261</v>
-      </c>
       <c r="D54" t="s">
+        <v>259</v>
+      </c>
+      <c r="E54" t="s">
         <v>260</v>
-      </c>
-      <c r="E54" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B55" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B56" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B57" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A58" s="8" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B58" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C58" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B59" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C59" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D59" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B60" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C60" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D60" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E60" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B61" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C61" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D61" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E61" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A62" s="7" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B62" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -4797,7 +4835,7 @@
   <dimension ref="A1:N43"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B9" sqref="B9:N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4811,16 +4849,16 @@
         <v>173</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>268</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
@@ -4828,40 +4866,40 @@
         <v>129</v>
       </c>
       <c r="B2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C2" t="s">
+        <v>262</v>
+      </c>
+      <c r="D2" t="s">
+        <v>275</v>
+      </c>
+      <c r="E2" t="s">
+        <v>275</v>
+      </c>
+      <c r="F2" t="s">
+        <v>275</v>
+      </c>
+      <c r="G2" t="s">
+        <v>275</v>
+      </c>
+      <c r="H2" t="s">
         <v>263</v>
       </c>
-      <c r="C2" t="s">
+      <c r="I2" t="s">
         <v>263</v>
       </c>
-      <c r="D2" t="s">
-        <v>276</v>
-      </c>
-      <c r="E2" t="s">
-        <v>276</v>
-      </c>
-      <c r="F2" t="s">
-        <v>276</v>
-      </c>
-      <c r="G2" t="s">
-        <v>276</v>
-      </c>
-      <c r="H2" t="s">
-        <v>264</v>
-      </c>
-      <c r="I2" t="s">
-        <v>264</v>
-      </c>
       <c r="J2" t="s">
+        <v>279</v>
+      </c>
+      <c r="K2" t="s">
         <v>280</v>
       </c>
-      <c r="K2" t="s">
-        <v>281</v>
-      </c>
       <c r="L2" s="13" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="N2" s="13"/>
     </row>
@@ -4870,34 +4908,34 @@
         <v>135</v>
       </c>
       <c r="B3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
@@ -4905,34 +4943,34 @@
         <v>126</v>
       </c>
       <c r="B4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H4" t="s">
+        <v>279</v>
+      </c>
+      <c r="I4" t="s">
         <v>280</v>
       </c>
-      <c r="I4" t="s">
-        <v>281</v>
-      </c>
       <c r="J4" s="13" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
@@ -4940,34 +4978,34 @@
         <v>132</v>
       </c>
       <c r="B5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H5" t="s">
+        <v>279</v>
+      </c>
+      <c r="I5" t="s">
         <v>280</v>
       </c>
-      <c r="I5" t="s">
-        <v>281</v>
-      </c>
       <c r="J5" s="13" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
@@ -4975,31 +5013,31 @@
         <v>138</v>
       </c>
       <c r="B6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -5007,10 +5045,10 @@
         <v>147</v>
       </c>
       <c r="B7" t="s">
+        <v>279</v>
+      </c>
+      <c r="C7" t="s">
         <v>280</v>
-      </c>
-      <c r="C7" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
@@ -5018,34 +5056,43 @@
         <v>141</v>
       </c>
       <c r="B8" t="s">
+        <v>262</v>
+      </c>
+      <c r="C8" t="s">
+        <v>262</v>
+      </c>
+      <c r="D8" t="s">
+        <v>275</v>
+      </c>
+      <c r="E8" t="s">
+        <v>275</v>
+      </c>
+      <c r="F8" t="s">
+        <v>275</v>
+      </c>
+      <c r="G8" t="s">
+        <v>275</v>
+      </c>
+      <c r="H8" t="s">
+        <v>275</v>
+      </c>
+      <c r="I8" t="s">
         <v>263</v>
       </c>
-      <c r="C8" t="s">
+      <c r="J8" t="s">
         <v>263</v>
       </c>
-      <c r="D8" t="s">
-        <v>276</v>
-      </c>
-      <c r="E8" t="s">
-        <v>276</v>
-      </c>
-      <c r="F8" t="s">
-        <v>264</v>
-      </c>
-      <c r="G8" t="s">
-        <v>264</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="K8" t="s">
+        <v>279</v>
+      </c>
+      <c r="L8" t="s">
         <v>280</v>
       </c>
-      <c r="I8" t="s">
-        <v>281</v>
-      </c>
-      <c r="J8" s="13" t="s">
-        <v>462</v>
-      </c>
-      <c r="K8" s="13" t="s">
-        <v>263</v>
+      <c r="M8" s="13" t="s">
+        <v>460</v>
+      </c>
+      <c r="N8" s="13" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
@@ -5053,100 +5100,109 @@
         <v>144</v>
       </c>
       <c r="B9" t="s">
+        <v>262</v>
+      </c>
+      <c r="C9" t="s">
+        <v>262</v>
+      </c>
+      <c r="D9" t="s">
+        <v>275</v>
+      </c>
+      <c r="E9" t="s">
+        <v>275</v>
+      </c>
+      <c r="F9" t="s">
+        <v>275</v>
+      </c>
+      <c r="G9" t="s">
+        <v>275</v>
+      </c>
+      <c r="H9" t="s">
+        <v>275</v>
+      </c>
+      <c r="I9" t="s">
         <v>263</v>
       </c>
-      <c r="C9" t="s">
+      <c r="J9" t="s">
         <v>263</v>
       </c>
-      <c r="D9" t="s">
-        <v>276</v>
-      </c>
-      <c r="E9" t="s">
-        <v>276</v>
-      </c>
-      <c r="F9" t="s">
-        <v>264</v>
-      </c>
-      <c r="G9" t="s">
-        <v>264</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="K9" t="s">
+        <v>279</v>
+      </c>
+      <c r="L9" t="s">
         <v>280</v>
       </c>
-      <c r="I9" t="s">
-        <v>281</v>
-      </c>
-      <c r="J9" s="13" t="s">
-        <v>462</v>
-      </c>
-      <c r="K9" s="13" t="s">
-        <v>263</v>
+      <c r="M9" s="13" t="s">
+        <v>460</v>
+      </c>
+      <c r="N9" s="13" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B10" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C11" t="s">
+        <v>269</v>
+      </c>
+      <c r="D11" t="s">
+        <v>262</v>
+      </c>
+      <c r="E11" t="s">
         <v>270</v>
       </c>
-      <c r="C11" t="s">
+      <c r="F11" t="s">
         <v>270</v>
-      </c>
-      <c r="D11" t="s">
-        <v>263</v>
-      </c>
-      <c r="E11" t="s">
-        <v>271</v>
-      </c>
-      <c r="F11" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B12" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C12" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D12" t="s">
+        <v>271</v>
+      </c>
+      <c r="E12" t="s">
         <v>272</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>273</v>
       </c>
-      <c r="F12" t="s">
-        <v>274</v>
-      </c>
       <c r="G12" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H12" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I12" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J12" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K12" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
@@ -5154,7 +5210,7 @@
         <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
@@ -5162,7 +5218,7 @@
         <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
@@ -5170,13 +5226,13 @@
         <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C15" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D15" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
@@ -5184,7 +5240,7 @@
         <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -5192,7 +5248,7 @@
         <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -5200,7 +5256,7 @@
         <v>61</v>
       </c>
       <c r="B18" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -5208,7 +5264,7 @@
         <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -5216,7 +5272,7 @@
         <v>66</v>
       </c>
       <c r="B20" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -5224,7 +5280,7 @@
         <v>68</v>
       </c>
       <c r="B21" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -5232,7 +5288,7 @@
         <v>74</v>
       </c>
       <c r="B22" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -5240,7 +5296,7 @@
         <v>124</v>
       </c>
       <c r="B23" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -5248,7 +5304,7 @@
         <v>75</v>
       </c>
       <c r="B24" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -5256,7 +5312,7 @@
         <v>78</v>
       </c>
       <c r="B25" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
@@ -5264,7 +5320,7 @@
         <v>87</v>
       </c>
       <c r="B26" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
@@ -5272,7 +5328,7 @@
         <v>90</v>
       </c>
       <c r="B27" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
@@ -5280,7 +5336,7 @@
         <v>93</v>
       </c>
       <c r="B28" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
@@ -5288,7 +5344,7 @@
         <v>96</v>
       </c>
       <c r="B29" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
@@ -5296,7 +5352,7 @@
         <v>99</v>
       </c>
       <c r="B30" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
@@ -5304,7 +5360,7 @@
         <v>102</v>
       </c>
       <c r="B31" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -5312,7 +5368,7 @@
         <v>105</v>
       </c>
       <c r="B32" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.35">
@@ -5320,7 +5376,7 @@
         <v>108</v>
       </c>
       <c r="B33" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.35">
@@ -5328,7 +5384,7 @@
         <v>115</v>
       </c>
       <c r="B34" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.35">
@@ -5336,7 +5392,7 @@
         <v>118</v>
       </c>
       <c r="B35" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.35">
@@ -5344,135 +5400,135 @@
         <v>121</v>
       </c>
       <c r="B36" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37" s="7" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B37" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B38" t="s">
+        <v>262</v>
+      </c>
+      <c r="C38" t="s">
+        <v>262</v>
+      </c>
+      <c r="D38" t="s">
+        <v>275</v>
+      </c>
+      <c r="E38" t="s">
+        <v>275</v>
+      </c>
+      <c r="F38" t="s">
+        <v>275</v>
+      </c>
+      <c r="G38" t="s">
+        <v>275</v>
+      </c>
+      <c r="H38" t="s">
+        <v>275</v>
+      </c>
+      <c r="I38" t="s">
+        <v>275</v>
+      </c>
+      <c r="J38" t="s">
+        <v>275</v>
+      </c>
+      <c r="K38" t="s">
         <v>263</v>
       </c>
-      <c r="C38" t="s">
-        <v>263</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="L38" t="s">
+        <v>262</v>
+      </c>
+      <c r="M38" t="s">
         <v>276</v>
       </c>
-      <c r="E38" t="s">
-        <v>276</v>
-      </c>
-      <c r="F38" t="s">
-        <v>276</v>
-      </c>
-      <c r="G38" t="s">
-        <v>276</v>
-      </c>
-      <c r="H38" t="s">
-        <v>276</v>
-      </c>
-      <c r="I38" t="s">
-        <v>276</v>
-      </c>
-      <c r="J38" t="s">
-        <v>276</v>
-      </c>
-      <c r="K38" t="s">
-        <v>264</v>
-      </c>
-      <c r="L38" t="s">
-        <v>263</v>
-      </c>
-      <c r="M38" t="s">
-        <v>277</v>
-      </c>
       <c r="N38" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B39" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C39" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D39" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E39" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A40" s="8" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B40" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C40" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B41" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C41" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D41" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B42" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C42" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D42" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E42" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B43" t="s">
+        <v>262</v>
+      </c>
+      <c r="C43" t="s">
+        <v>262</v>
+      </c>
+      <c r="D43" t="s">
+        <v>275</v>
+      </c>
+      <c r="E43" t="s">
         <v>263</v>
-      </c>
-      <c r="C43" t="s">
-        <v>263</v>
-      </c>
-      <c r="D43" t="s">
-        <v>276</v>
-      </c>
-      <c r="E43" t="s">
-        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -5493,10 +5549,10 @@
   </sheetPr>
   <dimension ref="A1:W54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection activeCell="A34" sqref="A34"/>
-      <selection pane="topRight" activeCell="B20" sqref="B20"/>
+      <selection pane="topRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5514,7 +5570,7 @@
     <col min="12" max="12" width="23.90625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.6328125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21" customWidth="1"/>
     <col min="16" max="16" width="15.1796875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15.08984375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="21.90625" bestFit="1" customWidth="1"/>
@@ -5530,31 +5586,31 @@
         <v>173</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>286</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>290</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
@@ -5562,43 +5618,43 @@
         <v>129</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C2" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>343</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>344</v>
-      </c>
       <c r="E2" t="s">
+        <v>351</v>
+      </c>
+      <c r="F2" t="s">
         <v>352</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>353</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" s="13" t="s">
         <v>354</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="I2" s="13" t="s">
         <v>355</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="J2" s="13" t="s">
         <v>356</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="K2" s="13" t="s">
+        <v>345</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="M2" s="13" t="s">
         <v>357</v>
       </c>
-      <c r="K2" s="13" t="s">
-        <v>346</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>347</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>358</v>
-      </c>
       <c r="N2" s="13" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="O2" s="13"/>
       <c r="P2" s="13"/>
@@ -5609,22 +5665,22 @@
         <v>150</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D3" s="13" t="s">
+        <v>364</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>365</v>
+      </c>
+      <c r="F3" s="13" t="s">
         <v>366</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="G3" s="13" t="s">
         <v>367</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>368</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
@@ -5632,22 +5688,22 @@
         <v>153</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D4" t="s">
+        <v>368</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>369</v>
+      </c>
+      <c r="F4" s="13" t="s">
         <v>370</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="G4" s="13" t="s">
         <v>371</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>372</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
@@ -5655,37 +5711,37 @@
         <v>135</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C5" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>343</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>344</v>
-      </c>
       <c r="E5" s="13" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>361</v>
+        <v>472</v>
       </c>
       <c r="G5" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>457</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>459</v>
+      </c>
+      <c r="L5" s="13" t="s">
         <v>350</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>459</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>359</v>
-      </c>
-      <c r="J5" s="13" t="s">
-        <v>360</v>
-      </c>
-      <c r="K5" s="13" t="s">
-        <v>461</v>
-      </c>
-      <c r="L5" s="13" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
@@ -5693,37 +5749,37 @@
         <v>126</v>
       </c>
       <c r="B6" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C6" t="s">
+        <v>342</v>
+      </c>
+      <c r="D6" t="s">
         <v>343</v>
       </c>
-      <c r="D6" t="s">
-        <v>344</v>
-      </c>
       <c r="E6" t="s">
+        <v>347</v>
+      </c>
+      <c r="F6" t="s">
         <v>348</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" s="13" t="s">
         <v>349</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="H6" t="s">
+        <v>457</v>
+      </c>
+      <c r="I6" t="s">
+        <v>345</v>
+      </c>
+      <c r="J6" t="s">
+        <v>346</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>459</v>
+      </c>
+      <c r="L6" s="13" t="s">
         <v>350</v>
-      </c>
-      <c r="H6" t="s">
-        <v>459</v>
-      </c>
-      <c r="I6" t="s">
-        <v>346</v>
-      </c>
-      <c r="J6" t="s">
-        <v>347</v>
-      </c>
-      <c r="K6" s="13" t="s">
-        <v>461</v>
-      </c>
-      <c r="L6" s="13" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
@@ -5731,37 +5787,37 @@
         <v>132</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C7" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>343</v>
       </c>
-      <c r="D7" s="13" t="s">
-        <v>344</v>
-      </c>
       <c r="E7" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="F7" s="13" t="s">
         <v>348</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="G7" s="13" t="s">
         <v>349</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="H7" s="13" t="s">
+        <v>457</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>345</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>459</v>
+      </c>
+      <c r="L7" s="13" t="s">
         <v>350</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>459</v>
-      </c>
-      <c r="I7" s="13" t="s">
-        <v>346</v>
-      </c>
-      <c r="J7" s="13" t="s">
-        <v>347</v>
-      </c>
-      <c r="K7" s="13" t="s">
-        <v>461</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>351</v>
       </c>
       <c r="M7" s="13"/>
       <c r="N7" s="13"/>
@@ -5771,34 +5827,34 @@
         <v>138</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C8" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="D8" s="13" t="s">
         <v>343</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="E8" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>457</v>
+      </c>
+      <c r="H8" s="13" t="s">
         <v>344</v>
       </c>
-      <c r="E8" s="13" t="s">
-        <v>348</v>
-      </c>
-      <c r="F8" s="13" t="s">
+      <c r="I8" s="13" t="s">
+        <v>345</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>459</v>
+      </c>
+      <c r="K8" s="13" t="s">
         <v>350</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>459</v>
-      </c>
-      <c r="H8" s="13" t="s">
-        <v>345</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>346</v>
-      </c>
-      <c r="J8" s="13" t="s">
-        <v>461</v>
-      </c>
-      <c r="K8" s="13" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.35">
@@ -5806,13 +5862,13 @@
         <v>147</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D9" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.35">
@@ -5820,37 +5876,46 @@
         <v>141</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C10" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="D10" s="13" t="s">
         <v>343</v>
       </c>
-      <c r="D10" s="13" t="s">
-        <v>344</v>
-      </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" t="s">
+        <v>351</v>
+      </c>
+      <c r="F10" t="s">
+        <v>352</v>
+      </c>
+      <c r="G10" t="s">
+        <v>353</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>471</v>
+      </c>
+      <c r="I10" s="13" t="s">
         <v>348</v>
       </c>
-      <c r="F10" s="13" t="s">
-        <v>349</v>
-      </c>
-      <c r="G10" s="13" t="s">
+      <c r="J10" s="13" t="s">
+        <v>355</v>
+      </c>
+      <c r="K10" s="13" t="s">
         <v>356</v>
       </c>
-      <c r="H10" s="13" t="s">
+      <c r="L10" s="13" t="s">
+        <v>345</v>
+      </c>
+      <c r="M10" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="N10" s="13" t="s">
         <v>357</v>
       </c>
-      <c r="I10" s="13" t="s">
-        <v>346</v>
-      </c>
-      <c r="J10" s="13" t="s">
-        <v>347</v>
-      </c>
-      <c r="K10" s="13" t="s">
-        <v>358</v>
-      </c>
-      <c r="L10" s="13" t="s">
-        <v>351</v>
+      <c r="O10" s="13" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.35">
@@ -5858,247 +5923,256 @@
         <v>144</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C11" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="D11" s="13" t="s">
         <v>343</v>
       </c>
-      <c r="D11" s="13" t="s">
-        <v>344</v>
-      </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" t="s">
+        <v>351</v>
+      </c>
+      <c r="F11" t="s">
+        <v>352</v>
+      </c>
+      <c r="G11" t="s">
+        <v>353</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>471</v>
+      </c>
+      <c r="I11" s="13" t="s">
         <v>348</v>
       </c>
-      <c r="F11" s="13" t="s">
-        <v>349</v>
-      </c>
-      <c r="G11" s="13" t="s">
+      <c r="J11" s="13" t="s">
+        <v>355</v>
+      </c>
+      <c r="K11" s="13" t="s">
         <v>356</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="L11" s="13" t="s">
+        <v>345</v>
+      </c>
+      <c r="M11" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="N11" s="13" t="s">
         <v>357</v>
       </c>
-      <c r="I11" s="13" t="s">
-        <v>346</v>
-      </c>
-      <c r="J11" s="13" t="s">
-        <v>347</v>
-      </c>
-      <c r="K11" s="13" t="s">
-        <v>358</v>
-      </c>
-      <c r="L11" s="13" t="s">
-        <v>351</v>
+      <c r="O11" s="13" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C12" s="12" t="s">
+        <v>307</v>
+      </c>
+      <c r="D12" t="s">
         <v>308</v>
-      </c>
-      <c r="D12" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C13" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="E13" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="F13" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="G13" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="H13" s="6" t="s">
         <v>314</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C14" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="E14" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="F14" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="G14" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="H14" s="6" t="s">
         <v>314</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D15" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="E15" s="12" t="s">
         <v>316</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C16" t="s">
+        <v>307</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="E16" t="s">
         <v>308</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="F16" t="s">
         <v>318</v>
       </c>
-      <c r="E16" t="s">
-        <v>309</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>319</v>
-      </c>
-      <c r="G16" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C17" t="s">
+        <v>320</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>321</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="E17" t="s">
         <v>322</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>323</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>324</v>
-      </c>
-      <c r="G17" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C18" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D18" t="s">
+        <v>325</v>
+      </c>
+      <c r="E18" t="s">
         <v>326</v>
-      </c>
-      <c r="E18" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C19" t="s">
+        <v>327</v>
+      </c>
+      <c r="D19" t="s">
         <v>328</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>329</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>330</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>331</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>332</v>
-      </c>
-      <c r="H19" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C20" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="D20" s="12" t="s">
         <v>334</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="E20" s="12" t="s">
         <v>335</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="F20" s="12" t="s">
         <v>336</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="G20" s="12" t="s">
         <v>337</v>
       </c>
-      <c r="G20" s="12" t="s">
+      <c r="H20" s="12" t="s">
         <v>338</v>
       </c>
-      <c r="H20" s="12" t="s">
+      <c r="I20" s="12" t="s">
         <v>339</v>
       </c>
-      <c r="I20" s="12" t="s">
+      <c r="J20" s="12" t="s">
         <v>340</v>
       </c>
-      <c r="J20" s="12" t="s">
+      <c r="K20" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="L20" s="12" t="s">
         <v>341</v>
-      </c>
-      <c r="K20" s="12" t="s">
-        <v>299</v>
-      </c>
-      <c r="L20" s="12" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.35">
@@ -6106,10 +6180,10 @@
         <v>32</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
@@ -6117,10 +6191,10 @@
         <v>36</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C22" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.35">
@@ -6128,10 +6202,10 @@
         <v>39</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C23" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.35">
@@ -6139,10 +6213,10 @@
         <v>42</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C24" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.35">
@@ -6150,10 +6224,10 @@
         <v>48</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C25" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.35">
@@ -6161,10 +6235,10 @@
         <v>51</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C26" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.35">
@@ -6172,10 +6246,10 @@
         <v>55</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C27" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.35">
@@ -6183,10 +6257,10 @@
         <v>58</v>
       </c>
       <c r="B28" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C28" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.35">
@@ -6194,10 +6268,10 @@
         <v>61</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C29" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.35">
@@ -6205,10 +6279,10 @@
         <v>64</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C30" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.35">
@@ -6216,10 +6290,10 @@
         <v>66</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C31" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.35">
@@ -6227,10 +6301,10 @@
         <v>68</v>
       </c>
       <c r="B32" s="11" t="s">
+        <v>447</v>
+      </c>
+      <c r="C32" t="s">
         <v>449</v>
-      </c>
-      <c r="C32" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.35">
@@ -6238,10 +6312,10 @@
         <v>71</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C33" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.35">
@@ -6249,10 +6323,10 @@
         <v>74</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C34" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.35">
@@ -6260,10 +6334,10 @@
         <v>124</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C35" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.35">
@@ -6271,10 +6345,10 @@
         <v>165</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C36" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.35">
@@ -6282,10 +6356,10 @@
         <v>75</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C37" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.35">
@@ -6293,10 +6367,10 @@
         <v>78</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C38" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.35">
@@ -6304,21 +6378,21 @@
         <v>81</v>
       </c>
       <c r="B39" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C39" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="40" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B40" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C40" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D40"/>
       <c r="E40"/>
@@ -6340,10 +6414,10 @@
         <v>87</v>
       </c>
       <c r="B41" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C41" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.35">
@@ -6351,10 +6425,10 @@
         <v>90</v>
       </c>
       <c r="B42" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C42" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.35">
@@ -6362,10 +6436,10 @@
         <v>93</v>
       </c>
       <c r="B43" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C43" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.35">
@@ -6373,10 +6447,10 @@
         <v>96</v>
       </c>
       <c r="B44" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C44" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.35">
@@ -6384,10 +6458,10 @@
         <v>99</v>
       </c>
       <c r="B45" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C45" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.35">
@@ -6395,10 +6469,10 @@
         <v>102</v>
       </c>
       <c r="B46" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C46" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.35">
@@ -6406,10 +6480,10 @@
         <v>105</v>
       </c>
       <c r="B47" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C47" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.35">
@@ -6417,21 +6491,21 @@
         <v>108</v>
       </c>
       <c r="B48" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C48" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B49" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C49" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="U49" s="13"/>
       <c r="V49" s="13"/>
@@ -6529,22 +6603,22 @@
         <v>173</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>374</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>375</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>376</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>377</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>378</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -6552,10 +6626,10 @@
         <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -6563,10 +6637,10 @@
         <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C3" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -6574,10 +6648,10 @@
         <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C4" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -6585,22 +6659,22 @@
         <v>48</v>
       </c>
       <c r="B5" t="s">
+        <v>384</v>
+      </c>
+      <c r="C5" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5" t="s">
         <v>386</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>387</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>388</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>389</v>
-      </c>
-      <c r="F5" t="s">
-        <v>390</v>
-      </c>
-      <c r="G5" t="s">
-        <v>391</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reorder moorings module inputs
</commit_message>
<xml_diff>
--- a/dds/moorings.xlsx
+++ b/dds/moorings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="530" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="530"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1259" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1259" uniqueCount="475">
   <si>
     <t>Identifier</t>
   </si>
@@ -1458,19 +1458,29 @@
   </si>
   <si>
     <t>wet_mass</t>
+  </si>
+  <si>
+    <t>Soil Properties Table</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1619,28 +1629,28 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1650,16 +1660,17 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="40% - Accent3" xfId="2" builtinId="39"/>
@@ -2016,9 +2027,9 @@
   </sheetPr>
   <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2327,8 +2338,8 @@
       <c r="B20" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="15" t="s">
-        <v>27</v>
+      <c r="C20" s="24" t="s">
+        <v>474</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>27</v>
@@ -5559,7 +5570,7 @@
   </sheetPr>
   <dimension ref="A1:W54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
       <selection activeCell="A34" sqref="A34"/>
       <selection pane="topRight" activeCell="I2" sqref="I2"/>

</xml_diff>

<commit_message>
Change predefined foundations variable to preferred foundation and add option to repeat a single foundation design for each device.
</commit_message>
<xml_diff>
--- a/dds/moorings.xlsx
+++ b/dds/moorings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,10 +22,15 @@
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Types!$A$1:$U$62</definedName>
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Units!$A$1:$U$43</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">ROOT!$A$1:$H$64</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">ROOT!$A$1:$H$64</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Labels!$A$1:$P$25</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">Labels!$A$1:$P$25</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Types!$A$1:$U$62</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">Types!$A$1:$U$62</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Units!$A$1:$U$43</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Units!$A$1:$U$43</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">Tables!$A$1:$Q$48</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">Tables!$A$1:$Q$48</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -37,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1265" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1271" uniqueCount="481">
   <si>
     <t xml:space="preserve">Identifier</t>
   </si>
@@ -294,10 +299,10 @@
     <t xml:space="preserve">device.foundation_type</t>
   </si>
   <si>
-    <t xml:space="preserve">Foundation Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Predefined foundation type</t>
+    <t xml:space="preserve">Preferred Foundation Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preferred foundation type</t>
   </si>
   <si>
     <t xml:space="preserve">device.maximum_displacement</t>
@@ -691,6 +696,15 @@
   </si>
   <si>
     <t xml:space="preserve">Ignore single device forces calculated by the hydrodynamics module and use internal estimation instead</t>
+  </si>
+  <si>
+    <t xml:space="preserve">options.repeat_foundations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use Repeated Foundations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use a single foundation design per device for all foundation locations. This does not apply where a device has mixed foundation types.</t>
   </si>
   <si>
     <t xml:space="preserve">ID</t>
@@ -1517,18 +1531,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC5E0B4"/>
-        <bgColor rgb="FFDBDBDB"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1568,7 +1576,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1595,9 +1603,6 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1612,19 +1617,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1665,15 +1670,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in 40% - Accent6" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in 40% - Accent3" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1691,7 +1695,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC5E0B4"/>
+      <rgbColor rgb="FFDBDBDB"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -1711,7 +1715,7 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
@@ -1764,22 +1768,22 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H66"/>
+  <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B40" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
-      <selection pane="topRight" activeCell="A66" activeCellId="0" sqref="A66"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B19" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+      <selection pane="topRight" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="45.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="45.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="100.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1019" min="9" style="0" width="17.36"/>
@@ -2895,6 +2899,20 @@
       </c>
       <c r="D66" s="0" t="s">
         <v>217</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="D67" s="0" t="s">
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -2928,20 +2946,20 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="0" width="35.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="27.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="23.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="17.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="20.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="20.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="20.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="18.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="10.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="20.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="20.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="17.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="19.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="22" style="0" width="8.09"/>
@@ -2949,31 +2967,31 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2981,40 +2999,40 @@
         <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="Q2" s="10"/>
     </row>
@@ -3023,19 +3041,19 @@
         <v>12</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3043,19 +3061,19 @@
         <v>15</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3063,34 +3081,34 @@
         <v>18</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3098,34 +3116,34 @@
         <v>21</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3133,34 +3151,34 @@
         <v>24</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3168,31 +3186,31 @@
         <v>27</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3200,13 +3218,13 @@
         <v>30</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3214,43 +3232,43 @@
         <v>34</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="M10" s="9" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3258,43 +3276,43 @@
         <v>37</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="M11" s="9" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3302,10 +3320,10 @@
         <v>40</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3313,22 +3331,22 @@
         <v>44</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
@@ -3345,22 +3363,22 @@
         <v>48</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3368,13 +3386,13 @@
         <v>51</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3382,19 +3400,19 @@
         <v>54</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3402,19 +3420,19 @@
         <v>57</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3422,13 +3440,13 @@
         <v>60</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3436,22 +3454,22 @@
         <v>63</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3459,34 +3477,34 @@
         <v>66</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="J20" s="0" t="s">
         <v>160</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3494,43 +3512,43 @@
         <v>178</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="L21" s="0" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="M21" s="0" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="N21" s="0" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3538,16 +3556,16 @@
         <v>183</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3555,10 +3573,10 @@
         <v>195</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3566,13 +3584,13 @@
         <v>198</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3580,16 +3598,16 @@
         <v>201</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3597,16 +3615,16 @@
         <v>208</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -3628,10 +3646,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U63"/>
+  <dimension ref="A1:U64"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B63" activeCellId="0" sqref="B63"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B64" activeCellId="0" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3642,25 +3660,25 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3668,40 +3686,40 @@
         <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="O2" s="9"/>
       <c r="P2" s="9"/>
@@ -3712,19 +3730,19 @@
         <v>12</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3732,19 +3750,19 @@
         <v>15</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3752,34 +3770,34 @@
         <v>18</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="M5" s="9"/>
       <c r="N5" s="9"/>
@@ -3789,34 +3807,34 @@
         <v>21</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
@@ -3826,34 +3844,34 @@
         <v>24</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
@@ -3863,31 +3881,31 @@
         <v>27</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
@@ -3897,43 +3915,43 @@
         <v>34</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="N9" s="9" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3941,43 +3959,43 @@
         <v>37</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="M10" s="9" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3985,10 +4003,10 @@
         <v>40</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
@@ -4014,22 +4032,22 @@
         <v>44</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4037,22 +4055,22 @@
         <v>48</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4060,13 +4078,13 @@
         <v>51</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4074,19 +4092,19 @@
         <v>54</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4094,19 +4112,19 @@
         <v>57</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4114,13 +4132,13 @@
         <v>60</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4128,22 +4146,22 @@
         <v>63</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4151,34 +4169,34 @@
         <v>66</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4186,7 +4204,7 @@
         <v>69</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4194,7 +4212,7 @@
         <v>74</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4202,7 +4220,7 @@
         <v>77</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4210,7 +4228,7 @@
         <v>84</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4218,7 +4236,7 @@
         <v>87</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4226,7 +4244,7 @@
         <v>91</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4234,7 +4252,7 @@
         <v>94</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4242,7 +4260,7 @@
         <v>97</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4250,7 +4268,7 @@
         <v>100</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4258,7 +4276,7 @@
         <v>103</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4266,7 +4284,7 @@
         <v>106</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4274,7 +4292,7 @@
         <v>109</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4282,7 +4300,7 @@
         <v>113</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4290,7 +4308,7 @@
         <v>116</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4298,7 +4316,7 @@
         <v>119</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4306,7 +4324,7 @@
         <v>122</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4314,7 +4332,7 @@
         <v>125</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4322,7 +4340,7 @@
         <v>128</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4330,7 +4348,7 @@
         <v>132</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4338,7 +4356,7 @@
         <v>135</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4346,7 +4364,7 @@
         <v>138</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4354,7 +4372,7 @@
         <v>141</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4362,7 +4380,7 @@
         <v>144</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4370,7 +4388,7 @@
         <v>147</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4378,7 +4396,7 @@
         <v>150</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4386,7 +4404,7 @@
         <v>153</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4394,7 +4412,7 @@
         <v>156</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4402,7 +4420,7 @@
         <v>159</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4410,7 +4428,7 @@
         <v>162</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4418,7 +4436,7 @@
         <v>166</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4426,7 +4444,7 @@
         <v>169</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4434,7 +4452,7 @@
         <v>172</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4442,7 +4460,7 @@
         <v>175</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4450,43 +4468,43 @@
         <v>178</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="I53" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="J53" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="K53" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="L53" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="M53" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="N53" s="0" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4494,16 +4512,16 @@
         <v>183</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4511,7 +4529,7 @@
         <v>186</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4519,7 +4537,7 @@
         <v>189</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4527,7 +4545,7 @@
         <v>192</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4535,10 +4553,10 @@
         <v>195</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4546,13 +4564,13 @@
         <v>198</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4560,16 +4578,16 @@
         <v>201</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4577,16 +4595,16 @@
         <v>208</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4594,7 +4612,7 @@
         <v>211</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4602,7 +4620,15 @@
         <v>215</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>314</v>
+        <v>317</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -4632,25 +4658,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="17.36"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4658,40 +4684,40 @@
         <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="J2" s="0" t="s">
+        <v>326</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="M2" s="9" t="s">
         <v>323</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>324</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>325</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>320</v>
       </c>
       <c r="N2" s="9"/>
     </row>
@@ -4700,34 +4726,34 @@
         <v>18</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4735,34 +4761,34 @@
         <v>21</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="F4" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="H4" s="0" t="s">
         <v>326</v>
       </c>
-      <c r="G4" s="0" t="s">
-        <v>326</v>
-      </c>
-      <c r="H4" s="0" t="s">
+      <c r="I4" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="K4" s="9" t="s">
         <v>323</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>324</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>328</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4770,34 +4796,34 @@
         <v>24</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="F5" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="H5" s="0" t="s">
         <v>326</v>
       </c>
-      <c r="G5" s="0" t="s">
-        <v>326</v>
-      </c>
-      <c r="H5" s="0" t="s">
+      <c r="I5" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="K5" s="9" t="s">
         <v>323</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>324</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>328</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4805,31 +4831,31 @@
         <v>27</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="E6" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="H6" s="0" t="s">
         <v>326</v>
       </c>
-      <c r="F6" s="0" t="s">
-        <v>326</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>320</v>
-      </c>
-      <c r="H6" s="0" t="s">
+      <c r="I6" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="J6" s="9" t="s">
         <v>323</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>328</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4837,10 +4863,10 @@
         <v>30</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4848,43 +4874,43 @@
         <v>34</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="K8" s="0" t="s">
+        <v>326</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="M8" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="N8" s="9" t="s">
         <v>323</v>
-      </c>
-      <c r="L8" s="0" t="s">
-        <v>324</v>
-      </c>
-      <c r="M8" s="9" t="s">
-        <v>325</v>
-      </c>
-      <c r="N8" s="9" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4892,43 +4918,43 @@
         <v>37</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="K9" s="0" t="s">
+        <v>326</v>
+      </c>
+      <c r="L9" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="M9" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="N9" s="9" t="s">
         <v>323</v>
-      </c>
-      <c r="L9" s="0" t="s">
-        <v>324</v>
-      </c>
-      <c r="M9" s="9" t="s">
-        <v>325</v>
-      </c>
-      <c r="N9" s="9" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4936,10 +4962,10 @@
         <v>40</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4947,19 +4973,19 @@
         <v>54</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4967,34 +4993,34 @@
         <v>66</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5002,7 +5028,7 @@
         <v>74</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5010,7 +5036,7 @@
         <v>77</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5018,13 +5044,13 @@
         <v>80</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5032,7 +5058,7 @@
         <v>87</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5040,7 +5066,7 @@
         <v>94</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5048,7 +5074,7 @@
         <v>97</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5056,7 +5082,7 @@
         <v>100</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5064,7 +5090,7 @@
         <v>103</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5072,7 +5098,7 @@
         <v>106</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5080,7 +5106,7 @@
         <v>113</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5088,7 +5114,7 @@
         <v>116</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5096,7 +5122,7 @@
         <v>122</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5104,7 +5130,7 @@
         <v>125</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5112,7 +5138,7 @@
         <v>135</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5120,7 +5146,7 @@
         <v>138</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5128,7 +5154,7 @@
         <v>141</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5136,7 +5162,7 @@
         <v>144</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5144,7 +5170,7 @@
         <v>147</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5152,7 +5178,7 @@
         <v>150</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5160,7 +5186,7 @@
         <v>153</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5168,7 +5194,7 @@
         <v>156</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5176,7 +5202,7 @@
         <v>162</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5184,7 +5210,7 @@
         <v>166</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5192,7 +5218,7 @@
         <v>169</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5200,7 +5226,7 @@
         <v>172</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5208,43 +5234,43 @@
         <v>178</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="I38" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="J38" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="K38" s="0" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="L38" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="M38" s="0" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="N38" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5252,16 +5278,16 @@
         <v>183</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5269,10 +5295,10 @@
         <v>195</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5280,13 +5306,13 @@
         <v>198</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5294,16 +5320,16 @@
         <v>201</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5311,16 +5337,16 @@
         <v>208</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -5357,55 +5383,55 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="36.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="35.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="40.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="48.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="40.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="48.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="24.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="24.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="21.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="23.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="19.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="19.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="15.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="15.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="21.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="10.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="20.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="18.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="19.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="19.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="23" style="0" width="17.36"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5413,43 +5439,43 @@
         <v>8</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="O2" s="9"/>
       <c r="P2" s="9"/>
@@ -5460,22 +5486,22 @@
         <v>12</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5483,22 +5509,22 @@
         <v>15</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5506,37 +5532,37 @@
         <v>18</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5544,37 +5570,37 @@
         <v>21</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5582,37 +5608,37 @@
         <v>24</v>
       </c>
       <c r="B7" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>351</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>352</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>381</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>376</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="K7" s="9" t="s">
         <v>379</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>348</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>349</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>370</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>378</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>372</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>373</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>356</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>357</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>376</v>
-      </c>
       <c r="L7" s="9" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
@@ -5622,34 +5648,34 @@
         <v>27</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5657,13 +5683,13 @@
         <v>30</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5671,46 +5697,46 @@
         <v>34</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="M10" s="9" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="O10" s="9" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5718,46 +5744,46 @@
         <v>37</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="L11" s="9" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="M11" s="9" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="O11" s="9" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5765,13 +5791,13 @@
         <v>40</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5779,25 +5805,25 @@
         <v>44</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5805,25 +5831,25 @@
         <v>48</v>
       </c>
       <c r="B14" s="15" t="s">
+        <v>399</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>393</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>394</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="F14" s="10" t="s">
         <v>396</v>
       </c>
-      <c r="C14" s="10" t="s">
-        <v>390</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>391</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>392</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>393</v>
-      </c>
       <c r="G14" s="10" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5831,16 +5857,16 @@
         <v>51</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5848,22 +5874,22 @@
         <v>54</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5871,22 +5897,22 @@
         <v>57</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5894,16 +5920,16 @@
         <v>60</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5911,25 +5937,25 @@
         <v>63</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5937,37 +5963,37 @@
         <v>66</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="I20" s="15" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="J20" s="15" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="K20" s="15" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="L20" s="15" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5975,10 +6001,10 @@
         <v>69</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5986,10 +6012,10 @@
         <v>74</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5997,10 +6023,10 @@
         <v>77</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6008,10 +6034,10 @@
         <v>80</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6019,10 +6045,10 @@
         <v>84</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6030,10 +6056,10 @@
         <v>87</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6041,10 +6067,10 @@
         <v>91</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6052,10 +6078,10 @@
         <v>94</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6063,10 +6089,10 @@
         <v>97</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6074,10 +6100,10 @@
         <v>100</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6085,10 +6111,10 @@
         <v>103</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6096,10 +6122,10 @@
         <v>106</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6107,10 +6133,10 @@
         <v>109</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6118,10 +6144,10 @@
         <v>113</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6129,10 +6155,10 @@
         <v>116</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6140,10 +6166,10 @@
         <v>119</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6151,10 +6177,10 @@
         <v>122</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6162,10 +6188,10 @@
         <v>125</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6173,10 +6199,10 @@
         <v>128</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
     </row>
     <row r="40" s="9" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6184,10 +6210,10 @@
         <v>132</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6195,10 +6221,10 @@
         <v>135</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6206,10 +6232,10 @@
         <v>138</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6217,10 +6243,10 @@
         <v>141</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6228,10 +6254,10 @@
         <v>144</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6239,10 +6265,10 @@
         <v>147</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6250,10 +6276,10 @@
         <v>150</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6261,10 +6287,10 @@
         <v>153</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6272,10 +6298,10 @@
         <v>156</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6283,10 +6309,10 @@
         <v>159</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="U49" s="9"/>
       <c r="V49" s="9"/>
@@ -6319,31 +6345,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="17.36"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6351,10 +6377,10 @@
         <v>128</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6362,10 +6388,10 @@
         <v>109</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6373,10 +6399,10 @@
         <v>91</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6384,22 +6410,22 @@
         <v>84</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix predefined umbilical cable description
</commit_message>
<xml_diff>
--- a/dds/moorings.xlsx
+++ b/dds/moorings.xlsx
@@ -23,14 +23,19 @@
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Units!$A$1:$U$43</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">ROOT!$A$1:$H$64</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">ROOT!$A$1:$H$64</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">ROOT!$A$1:$H$64</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Labels!$A$1:$P$25</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">Labels!$A$1:$P$25</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Labels!$A$1:$P$25</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Types!$A$1:$U$62</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">Types!$A$1:$U$62</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Types!$A$1:$U$62</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Units!$A$1:$U$43</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Units!$A$1:$U$43</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Units!$A$1:$U$43</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">Tables!$A$1:$Q$48</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">Tables!$A$1:$Q$48</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Tables!$A$1:$Q$48</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -404,10 +409,10 @@
     <t xml:space="preserve">device.umbilical_type</t>
   </si>
   <si>
-    <t xml:space="preserve">Umbilical Cable Identifier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type of umbilical cable required for floating devices</t>
+    <t xml:space="preserve">Predefined Umbilical Cable Identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Predefined umbilical cable identifier</t>
   </si>
   <si>
     <t xml:space="preserve">device.wet_beam_area</t>
@@ -1770,10 +1775,10 @@
   </sheetPr>
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B19" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
-      <selection pane="topRight" activeCell="C26" activeCellId="0" sqref="C26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B25" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+      <selection pane="topRight" activeCell="D36" activeCellId="0" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2946,7 +2951,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="0" width="35.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="24"/>
@@ -5390,7 +5395,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="21.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="23.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="19.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="19.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="15.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="15.09"/>
@@ -5398,7 +5403,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="10.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="20.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="18.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="19.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="19.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="23" style="0" width="17.36"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Add options.use_max_thrust variable and apply to moorings interface
</commit_message>
<xml_diff>
--- a/dds/moorings.xlsx
+++ b/dds/moorings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\Python\git\dtocean-core\dds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24C6FF42-748B-481A-B16B-C10FE816166E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45EB6F8-09BE-4416-87D0-918E532E93B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1276" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="485">
   <si>
     <t>Identifier</t>
   </si>
@@ -1494,6 +1494,15 @@
   </si>
   <si>
     <t>4…</t>
+  </si>
+  <si>
+    <t>options.use_max_thrust</t>
+  </si>
+  <si>
+    <t>Use Maximum Turbine Thrust</t>
+  </si>
+  <si>
+    <t>Use the maximum turbine thrust coefficient for extreme rotor loads calculations. Defaults to False.</t>
   </si>
 </sst>
 </file>
@@ -1997,12 +2006,12 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:H67"/>
+  <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A25" sqref="A25"/>
-      <selection pane="topRight" activeCell="A9" sqref="A9"/>
+      <selection pane="topRight" activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3142,6 +3151,20 @@
       </c>
       <c r="D67" t="s">
         <v>217</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>482</v>
+      </c>
+      <c r="B68" t="s">
+        <v>163</v>
+      </c>
+      <c r="C68" t="s">
+        <v>483</v>
+      </c>
+      <c r="D68" t="s">
+        <v>484</v>
       </c>
     </row>
   </sheetData>
@@ -3860,10 +3883,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:U65"/>
+  <dimension ref="A1:U66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4854,6 +4877,14 @@
         <v>215</v>
       </c>
       <c r="B65" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>482</v>
+      </c>
+      <c r="B66" t="s">
         <v>314</v>
       </c>
     </row>

</xml_diff>